<commit_message>
Bug fix to solar capital costs in BS calculations
</commit_message>
<xml_diff>
--- a/InputData/fuels/BS/BAU Subsidies.xlsx
+++ b/InputData/fuels/BS/BAU Subsidies.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\fuels\BS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-colorado\InputData\fuels\BS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1236,9 +1236,6 @@
     <t>offshore wind ($/MW)</t>
   </si>
   <si>
-    <t>Model output, due to endogenous learning</t>
-  </si>
-  <si>
     <t>Solar PV  - $/MW</t>
   </si>
   <si>
@@ -1915,6 +1912,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Petroleum Products (billion 2019 dollars)</t>
+  </si>
+  <si>
+    <t>See elec/CCaMC</t>
   </si>
 </sst>
 </file>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.45">
@@ -2933,12 +2933,12 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="44" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
@@ -3836,7 +3836,7 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5148,7 +5148,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="46" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C1" s="49">
         <v>2019</v>
@@ -5256,10 +5256,10 @@
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="48" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
@@ -5267,23 +5267,23 @@
     </row>
     <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="48" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48"/>
       <c r="G4" s="48" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="48" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48"/>
@@ -5291,11 +5291,11 @@
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="48" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="48" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
@@ -5305,7 +5305,7 @@
     <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="45" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>43</v>
@@ -5417,7 +5417,7 @@
         <v>45</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -5532,7 +5532,7 @@
     </row>
     <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="45" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B16" s="52" t="s">
         <v>48</v>
@@ -5639,7 +5639,7 @@
     </row>
     <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="45" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B17" s="52" t="s">
         <v>49</v>
@@ -5746,7 +5746,7 @@
     </row>
     <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="45" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B18" s="52" t="s">
         <v>50</v>
@@ -5853,7 +5853,7 @@
     </row>
     <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="45" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B19" s="52" t="s">
         <v>51</v>
@@ -5960,7 +5960,7 @@
     </row>
     <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="45" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B20" s="52" t="s">
         <v>52</v>
@@ -6067,7 +6067,7 @@
     </row>
     <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="45" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B21" s="52" t="s">
         <v>236</v>
@@ -6174,7 +6174,7 @@
     </row>
     <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="45" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B22" s="52" t="s">
         <v>53</v>
@@ -6281,7 +6281,7 @@
     </row>
     <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="45" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B23" s="52" t="s">
         <v>54</v>
@@ -6388,7 +6388,7 @@
     </row>
     <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="45" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B24" s="52" t="s">
         <v>55</v>
@@ -6495,7 +6495,7 @@
     </row>
     <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="45" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B25" s="51" t="s">
         <v>56</v>
@@ -6607,7 +6607,7 @@
     </row>
     <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="45" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B28" s="52" t="s">
         <v>58</v>
@@ -6714,7 +6714,7 @@
     </row>
     <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="45" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B29" s="52" t="s">
         <v>59</v>
@@ -6821,7 +6821,7 @@
     </row>
     <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="45" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B30" s="52" t="s">
         <v>64</v>
@@ -6928,10 +6928,10 @@
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="45" t="s">
+        <v>416</v>
+      </c>
+      <c r="B31" s="52" t="s">
         <v>417</v>
-      </c>
-      <c r="B31" s="52" t="s">
-        <v>418</v>
       </c>
       <c r="C31" s="53">
         <v>0.29147099999999998</v>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B32" s="51" t="s">
         <v>56</v>
@@ -7148,10 +7148,10 @@
     </row>
     <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="45" t="s">
+        <v>419</v>
+      </c>
+      <c r="B35" s="52" t="s">
         <v>420</v>
-      </c>
-      <c r="B35" s="52" t="s">
-        <v>421</v>
       </c>
       <c r="C35" s="53">
         <v>16.702090999999999</v>
@@ -7255,7 +7255,7 @@
     </row>
     <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="45" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B36" s="52" t="s">
         <v>64</v>
@@ -7362,7 +7362,7 @@
     </row>
     <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B37" s="52" t="s">
         <v>61</v>
@@ -7469,7 +7469,7 @@
     </row>
     <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B38" s="51" t="s">
         <v>56</v>
@@ -7577,10 +7577,10 @@
     <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="45" t="s">
+        <v>424</v>
+      </c>
+      <c r="B40" s="51" t="s">
         <v>425</v>
-      </c>
-      <c r="B40" s="51" t="s">
-        <v>426</v>
       </c>
       <c r="C40" s="55">
         <v>2.0051730000000001</v>
@@ -7690,10 +7690,10 @@
     </row>
     <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="45" t="s">
+        <v>426</v>
+      </c>
+      <c r="B43" s="52" t="s">
         <v>427</v>
-      </c>
-      <c r="B43" s="52" t="s">
-        <v>428</v>
       </c>
       <c r="C43" s="53">
         <v>38.035392999999999</v>
@@ -7797,7 +7797,7 @@
     </row>
     <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="45" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B44" s="52" t="s">
         <v>64</v>
@@ -7904,10 +7904,10 @@
     </row>
     <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="45" t="s">
+        <v>429</v>
+      </c>
+      <c r="B45" s="52" t="s">
         <v>430</v>
-      </c>
-      <c r="B45" s="52" t="s">
-        <v>431</v>
       </c>
       <c r="C45" s="53">
         <v>11.249905999999999</v>
@@ -8011,7 +8011,7 @@
     </row>
     <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="45" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B46" s="52" t="s">
         <v>52</v>
@@ -8118,7 +8118,7 @@
     </row>
     <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B47" s="52" t="s">
         <v>236</v>
@@ -8225,10 +8225,10 @@
     </row>
     <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="45" t="s">
+        <v>433</v>
+      </c>
+      <c r="B48" s="52" t="s">
         <v>434</v>
-      </c>
-      <c r="B48" s="52" t="s">
-        <v>435</v>
       </c>
       <c r="C48" s="53">
         <v>3.2253970000000001</v>
@@ -8332,7 +8332,7 @@
     </row>
     <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B49" s="52" t="s">
         <v>54</v>
@@ -8439,10 +8439,10 @@
     </row>
     <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="45" t="s">
+        <v>436</v>
+      </c>
+      <c r="B50" s="52" t="s">
         <v>437</v>
-      </c>
-      <c r="B50" s="52" t="s">
-        <v>438</v>
       </c>
       <c r="C50" s="53">
         <v>0.28126800000000002</v>
@@ -8546,7 +8546,7 @@
     </row>
     <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="45" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B51" s="51" t="s">
         <v>65</v>
@@ -8654,12 +8654,12 @@
     <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="51" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="45" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B54" s="52" t="s">
         <v>66</v>
@@ -8766,7 +8766,7 @@
     </row>
     <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="45" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B55" s="52" t="s">
         <v>67</v>
@@ -8873,10 +8873,10 @@
     </row>
     <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="45" t="s">
+        <v>441</v>
+      </c>
+      <c r="B56" s="52" t="s">
         <v>442</v>
-      </c>
-      <c r="B56" s="52" t="s">
-        <v>443</v>
       </c>
       <c r="C56" s="53">
         <v>2.5672429999999999</v>
@@ -8980,10 +8980,10 @@
     </row>
     <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="45" t="s">
+        <v>443</v>
+      </c>
+      <c r="B57" s="52" t="s">
         <v>444</v>
-      </c>
-      <c r="B57" s="52" t="s">
-        <v>445</v>
       </c>
       <c r="C57" s="58">
         <v>34.304488999999997</v>
@@ -9087,10 +9087,10 @@
     </row>
     <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="45" t="s">
+        <v>445</v>
+      </c>
+      <c r="B58" s="52" t="s">
         <v>446</v>
-      </c>
-      <c r="B58" s="52" t="s">
-        <v>447</v>
       </c>
       <c r="C58" s="53">
         <v>1.7060120000000001</v>
@@ -9194,10 +9194,10 @@
     </row>
     <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="45" t="s">
+        <v>447</v>
+      </c>
+      <c r="B59" s="52" t="s">
         <v>448</v>
-      </c>
-      <c r="B59" s="52" t="s">
-        <v>449</v>
       </c>
       <c r="C59" s="53">
         <v>2.1898119999999999</v>
@@ -9301,7 +9301,7 @@
     </row>
     <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="45" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B60" s="52" t="s">
         <v>68</v>
@@ -9413,7 +9413,7 @@
     </row>
     <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="45" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B64" s="52" t="s">
         <v>66</v>
@@ -9520,7 +9520,7 @@
     </row>
     <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="45" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B65" s="52" t="s">
         <v>67</v>
@@ -9627,10 +9627,10 @@
     </row>
     <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="45" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B66" s="52" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C66" s="53">
         <v>2.5672429999999999</v>
@@ -9734,10 +9734,10 @@
     </row>
     <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="45" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B67" s="52" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C67" s="58">
         <v>34.304488999999997</v>
@@ -9841,10 +9841,10 @@
     </row>
     <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="45" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B68" s="52" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C68" s="53">
         <v>1.7060120000000001</v>
@@ -9948,10 +9948,10 @@
     </row>
     <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="45" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B69" s="52" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C69" s="53">
         <v>2.1898119999999999</v>
@@ -10055,7 +10055,7 @@
     </row>
     <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="45" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B70" s="52" t="s">
         <v>68</v>
@@ -10236,7 +10236,7 @@
     </row>
     <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B80" s="47" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10246,22 +10246,22 @@
     </row>
     <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B82" s="47" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B83" s="47" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B84" s="47" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B85" s="47" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="86" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10276,12 +10276,12 @@
     </row>
     <row r="88" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" s="47" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="89" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B89" s="47" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="90" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10291,12 +10291,12 @@
     </row>
     <row r="91" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B91" s="47" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="92" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B92" s="47" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="93" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10306,7 +10306,7 @@
     </row>
     <row r="94" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B94" s="47" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="95" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10316,7 +10316,7 @@
     </row>
     <row r="96" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B96" s="47" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10326,17 +10326,17 @@
     </row>
     <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B98" s="47" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B99" s="47" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B100" s="47" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -10386,7 +10386,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="46" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C1" s="49">
         <v>2019</v>
@@ -10494,10 +10494,10 @@
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="48" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
@@ -10505,23 +10505,23 @@
     </row>
     <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="48" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48"/>
       <c r="G4" s="48" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="48" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48"/>
@@ -10529,11 +10529,11 @@
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="48" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="48" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
@@ -10543,7 +10543,7 @@
     <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="45" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>138</v>
@@ -10655,7 +10655,7 @@
         <v>45</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -10781,7 +10781,7 @@
     </row>
     <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="45" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B19" s="52" t="s">
         <v>143</v>
@@ -10888,7 +10888,7 @@
     </row>
     <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="45" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B20" s="52" t="s">
         <v>144</v>
@@ -10995,7 +10995,7 @@
     </row>
     <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="45" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B21" s="52" t="s">
         <v>145</v>
@@ -11102,7 +11102,7 @@
     </row>
     <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="45" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B22" s="52" t="s">
         <v>146</v>
@@ -11209,7 +11209,7 @@
     </row>
     <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="45" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B23" s="52" t="s">
         <v>147</v>
@@ -11316,7 +11316,7 @@
     </row>
     <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B24" s="52" t="s">
         <v>148</v>
@@ -11423,7 +11423,7 @@
     </row>
     <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="45" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B25" s="52" t="s">
         <v>149</v>
@@ -11530,7 +11530,7 @@
     </row>
     <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="45" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B26" s="51" t="s">
         <v>150</v>
@@ -11642,7 +11642,7 @@
     </row>
     <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="45" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B28" s="52" t="s">
         <v>143</v>
@@ -11749,7 +11749,7 @@
     </row>
     <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="45" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B29" s="52" t="s">
         <v>144</v>
@@ -11856,7 +11856,7 @@
     </row>
     <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="45" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B30" s="52" t="s">
         <v>152</v>
@@ -11963,7 +11963,7 @@
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="45" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B31" s="52" t="s">
         <v>153</v>
@@ -12070,10 +12070,10 @@
     </row>
     <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="45" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C32" s="57">
         <v>0.22128500000000001</v>
@@ -12177,7 +12177,7 @@
     </row>
     <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="45" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B33" s="51" t="s">
         <v>150</v>
@@ -12284,7 +12284,7 @@
     </row>
     <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="45" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B34" s="51" t="s">
         <v>238</v>
@@ -12391,7 +12391,7 @@
     </row>
     <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="45" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B35" s="52" t="s">
         <v>154</v>
@@ -12499,7 +12499,7 @@
     <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B37" s="51" t="s">
         <v>155</v>
@@ -12612,7 +12612,7 @@
     </row>
     <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="45" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B40" s="52" t="s">
         <v>143</v>
@@ -12719,7 +12719,7 @@
     </row>
     <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="45" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B41" s="52" t="s">
         <v>144</v>
@@ -12826,7 +12826,7 @@
     </row>
     <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="45" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B42" s="52" t="s">
         <v>152</v>
@@ -12933,7 +12933,7 @@
     </row>
     <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="45" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B43" s="52" t="s">
         <v>157</v>
@@ -13040,7 +13040,7 @@
     </row>
     <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="45" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B44" s="52" t="s">
         <v>158</v>
@@ -13147,7 +13147,7 @@
     </row>
     <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="45" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B45" s="52" t="s">
         <v>159</v>
@@ -13254,7 +13254,7 @@
     </row>
     <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="45" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B46" s="51" t="s">
         <v>239</v>
@@ -13361,7 +13361,7 @@
     </row>
     <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="45" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B47" s="52" t="s">
         <v>160</v>
@@ -13468,7 +13468,7 @@
     </row>
     <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="45" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B48" s="51" t="s">
         <v>161</v>
@@ -13581,7 +13581,7 @@
     </row>
     <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="45" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B51" s="52" t="s">
         <v>143</v>
@@ -13688,7 +13688,7 @@
     </row>
     <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="45" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B52" s="52" t="s">
         <v>144</v>
@@ -13795,7 +13795,7 @@
     </row>
     <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="45" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B53" s="52" t="s">
         <v>152</v>
@@ -13902,7 +13902,7 @@
     </row>
     <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="45" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B54" s="52" t="s">
         <v>146</v>
@@ -14009,7 +14009,7 @@
     </row>
     <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="45" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B55" s="52" t="s">
         <v>162</v>
@@ -14116,7 +14116,7 @@
     </row>
     <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="45" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B56" s="52" t="s">
         <v>163</v>
@@ -14223,7 +14223,7 @@
     </row>
     <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="45" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B57" s="51" t="s">
         <v>241</v>
@@ -14330,7 +14330,7 @@
     </row>
     <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="45" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B58" s="51" t="s">
         <v>164</v>
@@ -14438,7 +14438,7 @@
     <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="45" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B60" s="51" t="s">
         <v>165</v>
@@ -14551,7 +14551,7 @@
     </row>
     <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="45" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B63" s="52" t="s">
         <v>167</v>
@@ -14658,7 +14658,7 @@
     </row>
     <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="45" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B64" s="52" t="s">
         <v>168</v>
@@ -14765,7 +14765,7 @@
     </row>
     <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B65" s="52" t="s">
         <v>169</v>
@@ -14872,7 +14872,7 @@
     </row>
     <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="45" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B66" s="52" t="s">
         <v>170</v>
@@ -14979,7 +14979,7 @@
     </row>
     <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="45" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B67" s="51" t="s">
         <v>171</v>
@@ -15086,7 +15086,7 @@
     </row>
     <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="45" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B68" s="52" t="s">
         <v>172</v>
@@ -15193,7 +15193,7 @@
     </row>
     <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="45" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B69" s="51" t="s">
         <v>173</v>
@@ -15306,12 +15306,12 @@
     </row>
     <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B72" s="51" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="73" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="45" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B73" s="52" t="s">
         <v>167</v>
@@ -15418,7 +15418,7 @@
     </row>
     <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="45" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B74" s="52" t="s">
         <v>168</v>
@@ -15525,7 +15525,7 @@
     </row>
     <row r="75" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="45" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B75" s="52" t="s">
         <v>169</v>
@@ -15632,7 +15632,7 @@
     </row>
     <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="45" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B76" s="52" t="s">
         <v>170</v>
@@ -15739,7 +15739,7 @@
     </row>
     <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="45" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B77" s="51" t="s">
         <v>175</v>
@@ -15851,7 +15851,7 @@
     </row>
     <row r="79" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="45" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B79" s="52" t="s">
         <v>167</v>
@@ -15958,7 +15958,7 @@
     </row>
     <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="45" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B80" s="52" t="s">
         <v>168</v>
@@ -16065,7 +16065,7 @@
     </row>
     <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="45" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B81" s="52" t="s">
         <v>169</v>
@@ -16172,7 +16172,7 @@
     </row>
     <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="45" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B82" s="52" t="s">
         <v>170</v>
@@ -16279,7 +16279,7 @@
     </row>
     <row r="83" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="45" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B83" s="51" t="s">
         <v>175</v>
@@ -16392,12 +16392,12 @@
     </row>
     <row r="86" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B86" s="51" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="87" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="45" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B87" s="52" t="s">
         <v>178</v>
@@ -16504,7 +16504,7 @@
     </row>
     <row r="88" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="45" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B88" s="52" t="s">
         <v>179</v>
@@ -16611,7 +16611,7 @@
     </row>
     <row r="89" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="45" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B89" s="52" t="s">
         <v>180</v>
@@ -16723,7 +16723,7 @@
     </row>
     <row r="91" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="45" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B91" s="52" t="s">
         <v>178</v>
@@ -16830,7 +16830,7 @@
     </row>
     <row r="92" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="45" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B92" s="52" t="s">
         <v>179</v>
@@ -16937,7 +16937,7 @@
     </row>
     <row r="93" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="45" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B93" s="52" t="s">
         <v>180</v>
@@ -17050,7 +17050,7 @@
     </row>
     <row r="96" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="45" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B96" s="52" t="s">
         <v>182</v>
@@ -17157,7 +17157,7 @@
     </row>
     <row r="97" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="45" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B97" s="52" t="s">
         <v>183</v>
@@ -17264,7 +17264,7 @@
     </row>
     <row r="98" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="45" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B98" s="52" t="s">
         <v>184</v>
@@ -17420,7 +17420,7 @@
     </row>
     <row r="103" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B103" s="47" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="104" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -17495,17 +17495,17 @@
     </row>
     <row r="118" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B118" s="47" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B119" s="47" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="120" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B120" s="47" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="121" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -17549,7 +17549,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="46" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C1" s="49">
         <v>2019</v>
@@ -17657,10 +17657,10 @@
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="48" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
@@ -17668,23 +17668,23 @@
     </row>
     <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="48" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48"/>
       <c r="G4" s="48" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="48" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48"/>
@@ -17692,11 +17692,11 @@
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="48" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="48" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
@@ -17706,7 +17706,7 @@
     <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="45" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>89</v>
@@ -17818,7 +17818,7 @@
         <v>45</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -17933,7 +17933,7 @@
     </row>
     <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="45" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B16" s="52" t="s">
         <v>93</v>
@@ -18040,7 +18040,7 @@
     </row>
     <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="45" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B17" s="52" t="s">
         <v>94</v>
@@ -18147,7 +18147,7 @@
     </row>
     <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="45" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B18" s="52" t="s">
         <v>95</v>
@@ -18254,7 +18254,7 @@
     </row>
     <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="45" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B19" s="52" t="s">
         <v>96</v>
@@ -18361,7 +18361,7 @@
     </row>
     <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="45" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B20" s="52" t="s">
         <v>97</v>
@@ -18468,7 +18468,7 @@
     </row>
     <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="45" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B21" s="52" t="s">
         <v>98</v>
@@ -18575,7 +18575,7 @@
     </row>
     <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="45" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B22" s="52" t="s">
         <v>99</v>
@@ -18682,7 +18682,7 @@
     </row>
     <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="45" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B23" s="51" t="s">
         <v>100</v>
@@ -18790,7 +18790,7 @@
     <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="45" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B25" s="52" t="s">
         <v>242</v>
@@ -18897,7 +18897,7 @@
     </row>
     <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="45" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B26" s="52" t="s">
         <v>243</v>
@@ -19004,7 +19004,7 @@
     </row>
     <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="45" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B27" s="52" t="s">
         <v>244</v>
@@ -19111,7 +19111,7 @@
     </row>
     <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="45" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B28" s="52" t="s">
         <v>245</v>
@@ -19218,7 +19218,7 @@
     </row>
     <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="45" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B29" s="52" t="s">
         <v>246</v>
@@ -19325,7 +19325,7 @@
     </row>
     <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="45" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B30" s="52" t="s">
         <v>247</v>
@@ -19432,7 +19432,7 @@
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="45" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B31" s="52" t="s">
         <v>248</v>
@@ -19539,7 +19539,7 @@
     </row>
     <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="45" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B32" s="52" t="s">
         <v>249</v>
@@ -19646,10 +19646,10 @@
     </row>
     <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="45" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C33" s="53">
         <v>1.0901460000000001</v>
@@ -19753,7 +19753,7 @@
     </row>
     <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="45" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B34" s="52" t="s">
         <v>250</v>
@@ -19860,7 +19860,7 @@
     </row>
     <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="45" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B35" s="52" t="s">
         <v>251</v>
@@ -19967,7 +19967,7 @@
     </row>
     <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="45" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B36" s="52" t="s">
         <v>252</v>
@@ -20074,7 +20074,7 @@
     </row>
     <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="45" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B37" s="52" t="s">
         <v>253</v>
@@ -20181,7 +20181,7 @@
     </row>
     <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="45" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B38" s="52" t="s">
         <v>254</v>
@@ -20288,7 +20288,7 @@
     </row>
     <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="45" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B39" s="52" t="s">
         <v>251</v>
@@ -20395,7 +20395,7 @@
     </row>
     <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="45" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B40" s="52" t="s">
         <v>252</v>
@@ -20502,7 +20502,7 @@
     </row>
     <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="45" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B41" s="52" t="s">
         <v>253</v>
@@ -20609,7 +20609,7 @@
     </row>
     <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="45" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B42" s="52" t="s">
         <v>255</v>
@@ -20716,7 +20716,7 @@
     </row>
     <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="45" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B43" s="52" t="s">
         <v>251</v>
@@ -20823,7 +20823,7 @@
     </row>
     <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="45" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B44" s="52" t="s">
         <v>252</v>
@@ -20930,7 +20930,7 @@
     </row>
     <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="45" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B45" s="52" t="s">
         <v>253</v>
@@ -21037,7 +21037,7 @@
     </row>
     <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="45" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B46" s="52" t="s">
         <v>256</v>
@@ -21144,7 +21144,7 @@
     </row>
     <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="45" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B47" s="52" t="s">
         <v>257</v>
@@ -21251,7 +21251,7 @@
     </row>
     <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="45" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B48" s="52" t="s">
         <v>258</v>
@@ -21359,7 +21359,7 @@
     <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="45" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B50" s="51" t="s">
         <v>101</v>
@@ -21478,7 +21478,7 @@
     </row>
     <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="45" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B55" s="52" t="s">
         <v>104</v>
@@ -21585,7 +21585,7 @@
     </row>
     <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="45" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B56" s="52" t="s">
         <v>105</v>
@@ -21692,7 +21692,7 @@
     </row>
     <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="45" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B57" s="52" t="s">
         <v>259</v>
@@ -21799,7 +21799,7 @@
     </row>
     <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="45" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B58" s="52" t="s">
         <v>106</v>
@@ -21906,7 +21906,7 @@
     </row>
     <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="45" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B59" s="52" t="s">
         <v>107</v>
@@ -22013,7 +22013,7 @@
     </row>
     <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="45" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B60" s="52" t="s">
         <v>108</v>
@@ -22120,7 +22120,7 @@
     </row>
     <row r="61" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="45" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B61" s="52" t="s">
         <v>109</v>
@@ -22227,7 +22227,7 @@
     </row>
     <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="45" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B62" s="52" t="s">
         <v>110</v>
@@ -22339,7 +22339,7 @@
     </row>
     <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="45" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B64" s="52" t="s">
         <v>112</v>
@@ -22446,7 +22446,7 @@
     </row>
     <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="45" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B65" s="52" t="s">
         <v>113</v>
@@ -22553,7 +22553,7 @@
     </row>
     <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="45" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B66" s="52" t="s">
         <v>114</v>
@@ -22660,7 +22660,7 @@
     </row>
     <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="45" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B67" s="52" t="s">
         <v>115</v>
@@ -22767,7 +22767,7 @@
     </row>
     <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="45" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B68" s="52" t="s">
         <v>260</v>
@@ -22874,7 +22874,7 @@
     </row>
     <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="45" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B69" s="51" t="s">
         <v>116</v>
@@ -22982,7 +22982,7 @@
     <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="71" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="45" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B71" s="52" t="s">
         <v>261</v>
@@ -23090,7 +23090,7 @@
     <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="73" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="45" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B73" s="52" t="s">
         <v>262</v>
@@ -23197,7 +23197,7 @@
     </row>
     <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="45" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B74" s="52" t="s">
         <v>263</v>
@@ -23304,10 +23304,10 @@
     </row>
     <row r="75" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="45" t="s">
+        <v>580</v>
+      </c>
+      <c r="B75" s="52" t="s">
         <v>581</v>
-      </c>
-      <c r="B75" s="52" t="s">
-        <v>582</v>
       </c>
       <c r="C75" s="53">
         <v>9.2183740000000007</v>
@@ -23411,10 +23411,10 @@
     </row>
     <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="45" t="s">
+        <v>582</v>
+      </c>
+      <c r="B76" s="52" t="s">
         <v>583</v>
-      </c>
-      <c r="B76" s="52" t="s">
-        <v>584</v>
       </c>
       <c r="C76" s="53">
         <v>8.7448569999999997</v>
@@ -23518,10 +23518,10 @@
     </row>
     <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="45" t="s">
+        <v>584</v>
+      </c>
+      <c r="B77" s="52" t="s">
         <v>585</v>
-      </c>
-      <c r="B77" s="52" t="s">
-        <v>586</v>
       </c>
       <c r="C77" s="53">
         <v>0.47351700000000002</v>
@@ -23625,7 +23625,7 @@
     </row>
     <row r="78" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="45" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B78" s="52" t="s">
         <v>117</v>
@@ -23737,10 +23737,10 @@
     </row>
     <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="45" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B80" s="52" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C80" s="57">
         <v>173.50422699999999</v>
@@ -23944,7 +23944,7 @@
     </row>
     <row r="96" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B96" s="47" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -23954,17 +23954,17 @@
     </row>
     <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B98" s="47" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B99" s="47" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B100" s="47" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -24009,17 +24009,17 @@
     </row>
     <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B109" s="47" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B110" s="47" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B111" s="47" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -24059,8 +24059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47:AH47"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -24116,7 +24116,7 @@
     </row>
     <row r="2" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="13"/>
@@ -24263,103 +24263,103 @@
         <v>304</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>395</v>
+        <v>621</v>
       </c>
       <c r="C4" s="7">
-        <v>1122140</v>
+        <v>1462790.2009077901</v>
       </c>
       <c r="D4" s="7">
-        <v>1093330</v>
+        <v>1284828.0428722501</v>
       </c>
       <c r="E4" s="7">
-        <v>1068540</v>
+        <v>1237544.2340474708</v>
       </c>
       <c r="F4" s="7">
-        <v>1046900</v>
+        <v>1190260.4252226916</v>
       </c>
       <c r="G4" s="7">
-        <v>1027790</v>
+        <v>1142976.6163979124</v>
       </c>
       <c r="H4" s="7">
-        <v>1010730</v>
+        <v>1095692.8075731331</v>
       </c>
       <c r="I4" s="8">
-        <v>995371</v>
+        <v>1048408.9987483537</v>
       </c>
       <c r="J4" s="8">
-        <v>979717</v>
+        <v>1001125.1899235747</v>
       </c>
       <c r="K4" s="8">
-        <v>965590</v>
+        <v>953841.38109879522</v>
       </c>
       <c r="L4" s="8">
-        <v>952751</v>
+        <v>906557.57227401587</v>
       </c>
       <c r="M4" s="8">
-        <v>941011</v>
+        <v>859273.76344923663</v>
       </c>
       <c r="N4" s="8">
-        <v>930219</v>
+        <v>811989.95462445728</v>
       </c>
       <c r="O4" s="8">
-        <v>920839</v>
+        <v>764706.14579967817</v>
       </c>
       <c r="P4" s="8">
-        <v>912101</v>
+        <v>757913.21727074252</v>
       </c>
       <c r="Q4" s="8">
-        <v>903931</v>
+        <v>751120.28874180699</v>
       </c>
       <c r="R4" s="8">
-        <v>896269</v>
+        <v>744327.36021287122</v>
       </c>
       <c r="S4" s="8">
-        <v>889064</v>
+        <v>737534.43168393557</v>
       </c>
       <c r="T4" s="8">
-        <v>881185</v>
+        <v>730741.50315499993</v>
       </c>
       <c r="U4" s="8">
-        <v>873806</v>
+        <v>723948.57462606428</v>
       </c>
       <c r="V4" s="8">
-        <v>866873</v>
+        <v>717155.64609712863</v>
       </c>
       <c r="W4" s="8">
-        <v>860342</v>
+        <v>710362.71756819298</v>
       </c>
       <c r="X4" s="8">
-        <v>854175</v>
+        <v>703569.78903925733</v>
       </c>
       <c r="Y4" s="8">
-        <v>848033</v>
+        <v>696776.86051032168</v>
       </c>
       <c r="Z4" s="8">
-        <v>842223</v>
+        <v>689983.93198138592</v>
       </c>
       <c r="AA4" s="8">
-        <v>836717</v>
+        <v>683191.00345245027</v>
       </c>
       <c r="AB4" s="8">
-        <v>831488</v>
+        <v>676398.07492351462</v>
       </c>
       <c r="AC4" s="8">
-        <v>826512</v>
+        <v>669605.14639457897</v>
       </c>
       <c r="AD4" s="8">
-        <v>821449</v>
+        <v>662812.21786564332</v>
       </c>
       <c r="AE4" s="8">
-        <v>816631</v>
+        <v>656019.28933670768</v>
       </c>
       <c r="AF4" s="8">
-        <v>812038</v>
+        <v>649226.36080777203</v>
       </c>
       <c r="AG4" s="8">
-        <v>807654</v>
+        <v>642433.43227883638</v>
       </c>
       <c r="AH4" s="8">
-        <v>803461</v>
+        <v>635640.50374990073</v>
       </c>
     </row>
     <row r="5" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
@@ -24501,137 +24501,137 @@
       </c>
       <c r="C6" s="31">
         <f t="shared" ref="C6:AH6" si="1">C5*C4</f>
-        <v>336642</v>
+        <v>438837.060272337</v>
       </c>
       <c r="D6" s="31">
         <f t="shared" si="1"/>
-        <v>284265.8</v>
+        <v>334055.29114678502</v>
       </c>
       <c r="E6" s="31">
         <f t="shared" si="1"/>
-        <v>235078.8</v>
+        <v>272259.73149044358</v>
       </c>
       <c r="F6" s="31">
         <f t="shared" si="1"/>
-        <v>104690</v>
+        <v>119026.04252226917</v>
       </c>
       <c r="G6" s="31">
         <f t="shared" si="1"/>
-        <v>102779</v>
+        <v>114297.66163979124</v>
       </c>
       <c r="H6" s="31">
         <f t="shared" si="1"/>
-        <v>101073</v>
+        <v>109569.28075731332</v>
       </c>
       <c r="I6" s="31">
         <f t="shared" si="1"/>
-        <v>99537.1</v>
+        <v>104840.89987483538</v>
       </c>
       <c r="J6" s="31">
         <f t="shared" si="1"/>
-        <v>97971.700000000012</v>
+        <v>100112.51899235748</v>
       </c>
       <c r="K6" s="31">
         <f t="shared" si="1"/>
-        <v>96559</v>
+        <v>95384.138109879525</v>
       </c>
       <c r="L6" s="31">
         <f t="shared" si="1"/>
-        <v>95275.1</v>
+        <v>90655.757227401598</v>
       </c>
       <c r="M6" s="31">
         <f t="shared" si="1"/>
-        <v>94101.1</v>
+        <v>85927.376344923672</v>
       </c>
       <c r="N6" s="31">
         <f t="shared" si="1"/>
-        <v>93021.900000000009</v>
+        <v>81198.995462445731</v>
       </c>
       <c r="O6" s="31">
         <f t="shared" si="1"/>
-        <v>92083.900000000009</v>
+        <v>76470.61457996782</v>
       </c>
       <c r="P6" s="31">
         <f t="shared" si="1"/>
-        <v>91210.1</v>
+        <v>75791.321727074261</v>
       </c>
       <c r="Q6" s="31">
         <f t="shared" si="1"/>
-        <v>90393.1</v>
+        <v>75112.028874180702</v>
       </c>
       <c r="R6" s="31">
         <f t="shared" si="1"/>
-        <v>89626.900000000009</v>
+        <v>74432.736021287128</v>
       </c>
       <c r="S6" s="31">
         <f t="shared" si="1"/>
-        <v>88906.400000000009</v>
+        <v>73753.443168393555</v>
       </c>
       <c r="T6" s="31">
         <f t="shared" si="1"/>
-        <v>88118.5</v>
+        <v>73074.150315499995</v>
       </c>
       <c r="U6" s="31">
         <f t="shared" si="1"/>
-        <v>87380.6</v>
+        <v>72394.857462606436</v>
       </c>
       <c r="V6" s="31">
         <f t="shared" si="1"/>
-        <v>86687.3</v>
+        <v>71715.564609712863</v>
       </c>
       <c r="W6" s="31">
         <f t="shared" si="1"/>
-        <v>86034.200000000012</v>
+        <v>71036.271756819304</v>
       </c>
       <c r="X6" s="31">
         <f t="shared" si="1"/>
-        <v>85417.5</v>
+        <v>70356.97890392573</v>
       </c>
       <c r="Y6" s="31">
         <f t="shared" si="1"/>
-        <v>84803.3</v>
+        <v>69677.686051032171</v>
       </c>
       <c r="Z6" s="31">
         <f t="shared" si="1"/>
-        <v>84222.3</v>
+        <v>68998.393198138598</v>
       </c>
       <c r="AA6" s="31">
         <f t="shared" si="1"/>
-        <v>83671.700000000012</v>
+        <v>68319.100345245024</v>
       </c>
       <c r="AB6" s="31">
         <f t="shared" si="1"/>
-        <v>83148.800000000003</v>
+        <v>67639.807492351465</v>
       </c>
       <c r="AC6" s="31">
         <f t="shared" si="1"/>
-        <v>82651.200000000012</v>
+        <v>66960.514639457906</v>
       </c>
       <c r="AD6" s="31">
         <f t="shared" si="1"/>
-        <v>82144.900000000009</v>
+        <v>66281.221786564332</v>
       </c>
       <c r="AE6" s="31">
         <f t="shared" si="1"/>
-        <v>81663.100000000006</v>
+        <v>65601.928933670773</v>
       </c>
       <c r="AF6" s="31">
         <f t="shared" si="1"/>
-        <v>81203.8</v>
+        <v>64922.636080777207</v>
       </c>
       <c r="AG6" s="31">
         <f t="shared" si="1"/>
-        <v>80765.400000000009</v>
+        <v>64243.343227883641</v>
       </c>
       <c r="AH6" s="31">
         <f t="shared" si="1"/>
-        <v>80346.100000000006</v>
+        <v>63564.050374990074</v>
       </c>
     </row>
     <row r="7" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="8" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="13"/>
@@ -24776,103 +24776,103 @@
         <v>308</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>395</v>
+        <v>621</v>
       </c>
       <c r="C10" s="7">
-        <v>3652290</v>
+        <v>6831836.4795198459</v>
       </c>
       <c r="D10" s="7">
-        <v>3497620</v>
+        <v>6500515.8491650894</v>
       </c>
       <c r="E10" s="7">
-        <v>3342950</v>
+        <v>6169195.2188103329</v>
       </c>
       <c r="F10" s="7">
-        <v>3270970</v>
+        <v>5843882.7444435377</v>
       </c>
       <c r="G10" s="7">
-        <v>3198990</v>
+        <v>5630238.7966989167</v>
       </c>
       <c r="H10" s="7">
-        <v>3127010</v>
+        <v>5422794.6290817559</v>
       </c>
       <c r="I10" s="7">
-        <v>3055030</v>
+        <v>5233450.6532794116</v>
       </c>
       <c r="J10" s="7">
-        <v>2983060</v>
+        <v>5058216.8964543967</v>
       </c>
       <c r="K10" s="7">
-        <v>2911080</v>
+        <v>4898609.074266511</v>
       </c>
       <c r="L10" s="7">
-        <v>2839100</v>
+        <v>4753976.9239266422</v>
       </c>
       <c r="M10" s="7">
-        <v>2767120</v>
+        <v>4620219.8524136795</v>
       </c>
       <c r="N10" s="7">
-        <v>2695140</v>
+        <v>4501029.6773458235</v>
       </c>
       <c r="O10" s="7">
-        <v>2623160</v>
+        <v>4393594.5403691512</v>
       </c>
       <c r="P10" s="7">
-        <v>2608110</v>
+        <v>4297491.1596871642</v>
       </c>
       <c r="Q10" s="7">
-        <v>2593050</v>
+        <v>4212533.3580054678</v>
       </c>
       <c r="R10" s="7">
-        <v>2577990</v>
+        <v>4135494.7609418505</v>
       </c>
       <c r="S10" s="7">
-        <v>2562930</v>
+        <v>4069499.8884631144</v>
       </c>
       <c r="T10" s="7">
-        <v>2547870</v>
+        <v>4010225.5494396384</v>
       </c>
       <c r="U10" s="7">
-        <v>2532810</v>
+        <v>3958592.5068339193</v>
       </c>
       <c r="V10" s="7">
-        <v>2517760</v>
+        <v>3914721.5043390612</v>
       </c>
       <c r="W10" s="7">
-        <v>2502700</v>
+        <v>3876446.5635061474</v>
       </c>
       <c r="X10" s="7">
-        <v>2487640</v>
+        <v>3843367.6747004823</v>
       </c>
       <c r="Y10" s="7">
-        <v>2472580</v>
+        <v>3814239.6224356443</v>
       </c>
       <c r="Z10" s="7">
-        <v>2457520</v>
+        <v>3789350.4384214408</v>
       </c>
       <c r="AA10" s="7">
-        <v>2442460</v>
+        <v>3768365.5466244677</v>
       </c>
       <c r="AB10" s="7">
-        <v>2427400</v>
+        <v>3749025.879948609</v>
       </c>
       <c r="AC10" s="7">
-        <v>2412350</v>
+        <v>3730662.2863270584</v>
       </c>
       <c r="AD10" s="7">
-        <v>2397290</v>
+        <v>3714585.4148475262</v>
       </c>
       <c r="AE10" s="7">
-        <v>2382230</v>
+        <v>3697197.8942802823</v>
       </c>
       <c r="AF10" s="7">
-        <v>2367170</v>
+        <v>3680144.9497464434</v>
       </c>
       <c r="AG10" s="7">
-        <v>2352110</v>
+        <v>3662115.9321582974</v>
       </c>
       <c r="AH10" s="7">
-        <v>2337050</v>
+        <v>3640824.119373824</v>
       </c>
     </row>
     <row r="11" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
@@ -25014,136 +25014,136 @@
       </c>
       <c r="C12" s="8">
         <f t="shared" ref="C12:AH12" si="3">C11*C10</f>
-        <v>1095687</v>
+        <v>2049550.9438559536</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="3"/>
-        <v>909381.20000000007</v>
+        <v>1690134.1207829234</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" si="3"/>
-        <v>735449</v>
+        <v>1357222.9481382733</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" si="3"/>
-        <v>327097</v>
+        <v>584388.27444435377</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" si="3"/>
-        <v>319899</v>
+        <v>563023.87966989167</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="3"/>
-        <v>312701</v>
+        <v>542279.46290817566</v>
       </c>
       <c r="I12" s="8">
         <f t="shared" si="3"/>
-        <v>305503</v>
+        <v>523345.06532794121</v>
       </c>
       <c r="J12" s="8">
         <f t="shared" si="3"/>
-        <v>298306</v>
+        <v>505821.68964543968</v>
       </c>
       <c r="K12" s="8">
         <f t="shared" si="3"/>
-        <v>291108</v>
+        <v>489860.9074266511</v>
       </c>
       <c r="L12" s="8">
         <f t="shared" si="3"/>
-        <v>283910</v>
+        <v>475397.69239266426</v>
       </c>
       <c r="M12" s="8">
         <f t="shared" si="3"/>
-        <v>276712</v>
+        <v>462021.98524136795</v>
       </c>
       <c r="N12" s="8">
         <f t="shared" si="3"/>
-        <v>269514</v>
+        <v>450102.96773458237</v>
       </c>
       <c r="O12" s="8">
         <f t="shared" si="3"/>
-        <v>262316</v>
+        <v>439359.45403691515</v>
       </c>
       <c r="P12" s="8">
         <f t="shared" si="3"/>
-        <v>260811</v>
+        <v>429749.11596871645</v>
       </c>
       <c r="Q12" s="8">
         <f t="shared" si="3"/>
-        <v>259305</v>
+        <v>421253.3358005468</v>
       </c>
       <c r="R12" s="8">
         <f t="shared" si="3"/>
-        <v>257799</v>
+        <v>413549.47609418508</v>
       </c>
       <c r="S12" s="8">
         <f t="shared" si="3"/>
-        <v>256293</v>
+        <v>406949.98884631146</v>
       </c>
       <c r="T12" s="8">
         <f t="shared" si="3"/>
-        <v>254787</v>
+        <v>401022.55494396389</v>
       </c>
       <c r="U12" s="8">
         <f t="shared" si="3"/>
-        <v>253281</v>
+        <v>395859.25068339193</v>
       </c>
       <c r="V12" s="8">
         <f t="shared" si="3"/>
-        <v>251776</v>
+        <v>391472.15043390612</v>
       </c>
       <c r="W12" s="8">
         <f t="shared" si="3"/>
-        <v>250270</v>
+        <v>387644.65635061474</v>
       </c>
       <c r="X12" s="8">
         <f t="shared" si="3"/>
-        <v>248764</v>
+        <v>384336.76747004827</v>
       </c>
       <c r="Y12" s="8">
         <f t="shared" si="3"/>
-        <v>247258</v>
+        <v>381423.96224356443</v>
       </c>
       <c r="Z12" s="8">
         <f t="shared" si="3"/>
-        <v>245752</v>
+        <v>378935.04384214408</v>
       </c>
       <c r="AA12" s="8">
         <f t="shared" si="3"/>
-        <v>244246</v>
+        <v>376836.55466244678</v>
       </c>
       <c r="AB12" s="8">
         <f t="shared" si="3"/>
-        <v>242740</v>
+        <v>374902.58799486095</v>
       </c>
       <c r="AC12" s="8">
         <f t="shared" si="3"/>
-        <v>241235</v>
+        <v>373066.22863270587</v>
       </c>
       <c r="AD12" s="8">
         <f t="shared" si="3"/>
-        <v>239729</v>
+        <v>371458.54148475267</v>
       </c>
       <c r="AE12" s="8">
         <f t="shared" si="3"/>
-        <v>238223</v>
+        <v>369719.78942802828</v>
       </c>
       <c r="AF12" s="8">
         <f t="shared" si="3"/>
-        <v>236717</v>
+        <v>368014.49497464439</v>
       </c>
       <c r="AG12" s="8">
         <f t="shared" si="3"/>
-        <v>235211</v>
+        <v>366211.59321582975</v>
       </c>
       <c r="AH12" s="8">
         <f t="shared" si="3"/>
-        <v>233705</v>
+        <v>364082.41193738242</v>
       </c>
     </row>
     <row r="14" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="13"/>
@@ -25656,7 +25656,7 @@
     <row r="19" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="20" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -26213,7 +26213,7 @@
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A26" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -33288,7 +33288,7 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
@@ -35223,7 +35223,7 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B18" s="28">
         <f>SUM(Calculations!C$69,Calculations!C$77,Calculations!C$85,Calculations!C$93,Calculations!C$100)</f>
@@ -35358,7 +35358,7 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B19" s="28">
         <f>SUM(Calculations!C$69,Calculations!C$77,Calculations!C$85,Calculations!C$93,Calculations!C$100)</f>
@@ -35493,7 +35493,7 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B20" s="6">
         <v>0</v>
@@ -35594,7 +35594,7 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B21" s="6">
         <v>0</v>
@@ -35695,7 +35695,7 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B22" s="6">
         <v>0</v>
@@ -35807,7 +35807,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -37431,7 +37431,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B15">
         <f>B11</f>
@@ -37566,7 +37566,7 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B16">
         <f>B11</f>
@@ -37701,7 +37701,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -38447,131 +38447,131 @@
       </c>
       <c r="B7" s="31">
         <f>(Calculations!C6)*(About!$A$70)</f>
-        <v>326879.38199999998</v>
+        <v>426110.78552443918</v>
       </c>
       <c r="C7" s="31">
         <f>(Calculations!D6)*(About!$A$70)</f>
-        <v>276022.09179999999</v>
+        <v>324367.68770352827</v>
       </c>
       <c r="D7" s="31">
         <f>(Calculations!E6)*(About!$A$70)</f>
-        <v>228261.51479999998</v>
+        <v>264364.1992772207</v>
       </c>
       <c r="E7" s="31">
         <f>(Calculations!F6)*(About!$A$70)</f>
-        <v>101653.98999999999</v>
+        <v>115574.28728912336</v>
       </c>
       <c r="F7" s="31">
         <f>(Calculations!G6)*(About!$A$70)</f>
-        <v>99798.409</v>
+        <v>110983.0294522373</v>
       </c>
       <c r="G7" s="31">
         <f>(Calculations!H6)*(About!$A$70)</f>
-        <v>98141.883000000002</v>
+        <v>106391.77161535123</v>
       </c>
       <c r="H7" s="31">
         <f>(Calculations!I6)*(About!$A$70)</f>
-        <v>96650.52410000001</v>
+        <v>101800.51377846515</v>
       </c>
       <c r="I7" s="31">
         <f>(Calculations!J6)*(About!$A$70)</f>
-        <v>95130.520700000008</v>
+        <v>97209.255941579104</v>
       </c>
       <c r="J7" s="31">
         <f>(Calculations!K6)*(About!$A$70)</f>
-        <v>93758.789000000004</v>
+        <v>92617.998104693019</v>
       </c>
       <c r="K7" s="31">
         <f>(Calculations!L6)*(About!$A$70)</f>
-        <v>92512.122100000008</v>
+        <v>88026.740267806948</v>
       </c>
       <c r="L7" s="31">
         <f>(Calculations!M6)*(About!$A$70)</f>
-        <v>91372.16810000001</v>
+        <v>83435.482430920878</v>
       </c>
       <c r="M7" s="31">
         <f>(Calculations!N6)*(About!$A$70)</f>
-        <v>90324.264900000009</v>
+        <v>78844.224594034808</v>
       </c>
       <c r="N7" s="31">
         <f>(Calculations!O6)*(About!$A$70)</f>
-        <v>89413.466899999999</v>
+        <v>74252.966757148752</v>
       </c>
       <c r="O7" s="31">
         <f>(Calculations!P6)*(About!$A$70)</f>
-        <v>88565.007100000003</v>
+        <v>73593.373396989104</v>
       </c>
       <c r="P7" s="31">
         <f>(Calculations!Q6)*(About!$A$70)</f>
-        <v>87771.700100000002</v>
+        <v>72933.780036829456</v>
       </c>
       <c r="Q7" s="31">
         <f>(Calculations!R6)*(About!$A$70)</f>
-        <v>87027.719900000011</v>
+        <v>72274.186676669793</v>
       </c>
       <c r="R7" s="31">
         <f>(Calculations!S6)*(About!$A$70)</f>
-        <v>86328.114400000006</v>
+        <v>71614.593316510145</v>
       </c>
       <c r="S7" s="31">
         <f>(Calculations!T6)*(About!$A$70)</f>
-        <v>85563.063500000004</v>
+        <v>70954.999956350497</v>
       </c>
       <c r="T7" s="31">
         <f>(Calculations!U6)*(About!$A$70)</f>
-        <v>84846.562600000005</v>
+        <v>70295.406596190849</v>
       </c>
       <c r="U7" s="31">
         <f>(Calculations!V6)*(About!$A$70)</f>
-        <v>84173.368300000002</v>
+        <v>69635.813236031187</v>
       </c>
       <c r="V7" s="31">
         <f>(Calculations!W6)*(About!$A$70)</f>
-        <v>83539.208200000008</v>
+        <v>68976.219875871539</v>
       </c>
       <c r="W7" s="31">
         <f>(Calculations!X6)*(About!$A$70)</f>
-        <v>82940.392500000002</v>
+        <v>68316.626515711876</v>
       </c>
       <c r="X7" s="31">
         <f>(Calculations!Y6)*(About!$A$70)</f>
-        <v>82344.004300000001</v>
+        <v>67657.033155552243</v>
       </c>
       <c r="Y7" s="31">
         <f>(Calculations!Z6)*(About!$A$70)</f>
-        <v>81779.853300000002</v>
+        <v>66997.43979539258</v>
       </c>
       <c r="Z7" s="31">
         <f>(Calculations!AA6)*(About!$A$70)</f>
-        <v>81245.220700000005</v>
+        <v>66337.846435232917</v>
       </c>
       <c r="AA7" s="31">
         <f>(Calculations!AB6)*(About!$A$70)</f>
-        <v>80737.484800000006</v>
+        <v>65678.253075073269</v>
       </c>
       <c r="AB7" s="31">
         <f>(Calculations!AC6)*(About!$A$70)</f>
-        <v>80254.315200000012</v>
+        <v>65018.659714913621</v>
       </c>
       <c r="AC7" s="31">
         <f>(Calculations!AD6)*(About!$A$70)</f>
-        <v>79762.697899999999</v>
+        <v>64359.066354753966</v>
       </c>
       <c r="AD7" s="31">
         <f>(Calculations!AE6)*(About!$A$70)</f>
-        <v>79294.8701</v>
+        <v>63699.472994594318</v>
       </c>
       <c r="AE7" s="31">
         <f>(Calculations!AF6)*(About!$A$70)</f>
-        <v>78848.889800000004</v>
+        <v>63039.879634434663</v>
       </c>
       <c r="AF7" s="31">
         <f>(Calculations!AG6)*(About!$A$70)</f>
-        <v>78423.203400000013</v>
+        <v>62380.286274275015</v>
       </c>
       <c r="AG7" s="31">
         <f>(Calculations!AH6)*(About!$A$70)</f>
-        <v>78016.063099999999</v>
+        <v>61720.69291411536</v>
       </c>
       <c r="AH7" s="31"/>
       <c r="AI7" s="31"/>
@@ -38582,131 +38582,131 @@
       </c>
       <c r="B8" s="31">
         <f>(Calculations!C12)*(About!$A$70)</f>
-        <v>1063912.077</v>
+        <v>1990113.9664841308</v>
       </c>
       <c r="C8" s="31">
         <f>(Calculations!D12)*(About!$A$70)</f>
-        <v>883009.14520000003</v>
+        <v>1641120.2312802186</v>
       </c>
       <c r="D8" s="31">
         <f>(Calculations!E12)*(About!$A$70)</f>
-        <v>714120.97899999993</v>
+        <v>1317863.4826422634</v>
       </c>
       <c r="E8" s="31">
         <f>(Calculations!F12)*(About!$A$70)</f>
-        <v>317611.18699999998</v>
+        <v>567441.01448546746</v>
       </c>
       <c r="F8" s="31">
         <f>(Calculations!G12)*(About!$A$70)</f>
-        <v>310621.929</v>
+        <v>546696.18715946481</v>
       </c>
       <c r="G8" s="31">
         <f>(Calculations!H12)*(About!$A$70)</f>
-        <v>303632.67099999997</v>
+        <v>526553.3584838385</v>
       </c>
       <c r="H8" s="31">
         <f>(Calculations!I12)*(About!$A$70)</f>
-        <v>296643.413</v>
+        <v>508168.05843343091</v>
       </c>
       <c r="I8" s="31">
         <f>(Calculations!J12)*(About!$A$70)</f>
-        <v>289655.12599999999</v>
+        <v>491152.8606457219</v>
       </c>
       <c r="J8" s="31">
         <f>(Calculations!K12)*(About!$A$70)</f>
-        <v>282665.86800000002</v>
+        <v>475654.9411112782</v>
       </c>
       <c r="K8" s="31">
         <f>(Calculations!L12)*(About!$A$70)</f>
-        <v>275676.61</v>
+        <v>461611.15931327699</v>
       </c>
       <c r="L8" s="31">
         <f>(Calculations!M12)*(About!$A$70)</f>
-        <v>268687.35200000001</v>
+        <v>448623.34766936826</v>
       </c>
       <c r="M8" s="31">
         <f>(Calculations!N12)*(About!$A$70)</f>
-        <v>261698.09399999998</v>
+        <v>437049.98167027946</v>
       </c>
       <c r="N8" s="31">
         <f>(Calculations!O12)*(About!$A$70)</f>
-        <v>254708.83599999998</v>
+        <v>426618.02986984461</v>
       </c>
       <c r="O8" s="31">
         <f>(Calculations!P12)*(About!$A$70)</f>
-        <v>253247.481</v>
+        <v>417286.39160562365</v>
       </c>
       <c r="P8" s="31">
         <f>(Calculations!Q12)*(About!$A$70)</f>
-        <v>251785.155</v>
+        <v>409036.98906233092</v>
       </c>
       <c r="Q8" s="31">
         <f>(Calculations!R12)*(About!$A$70)</f>
-        <v>250322.829</v>
+        <v>401556.54128745373</v>
       </c>
       <c r="R8" s="31">
         <f>(Calculations!S12)*(About!$A$70)</f>
-        <v>248860.503</v>
+        <v>395148.43916976842</v>
       </c>
       <c r="S8" s="31">
         <f>(Calculations!T12)*(About!$A$70)</f>
-        <v>247398.177</v>
+        <v>389392.90085058892</v>
       </c>
       <c r="T8" s="31">
         <f>(Calculations!U12)*(About!$A$70)</f>
-        <v>245935.851</v>
+        <v>384379.33241357357</v>
       </c>
       <c r="U8" s="31">
         <f>(Calculations!V12)*(About!$A$70)</f>
-        <v>244474.49599999998</v>
+        <v>380119.45807132282</v>
       </c>
       <c r="V8" s="31">
         <f>(Calculations!W12)*(About!$A$70)</f>
-        <v>243012.16999999998</v>
+        <v>376402.96131644689</v>
       </c>
       <c r="W8" s="31">
         <f>(Calculations!X12)*(About!$A$70)</f>
-        <v>241549.84399999998</v>
+        <v>373191.00121341686</v>
       </c>
       <c r="X8" s="31">
         <f>(Calculations!Y12)*(About!$A$70)</f>
-        <v>240087.51799999998</v>
+        <v>370362.66733850102</v>
       </c>
       <c r="Y8" s="31">
         <f>(Calculations!Z12)*(About!$A$70)</f>
-        <v>238625.19199999998</v>
+        <v>367945.92757072189</v>
       </c>
       <c r="Z8" s="31">
         <f>(Calculations!AA12)*(About!$A$70)</f>
-        <v>237162.86599999998</v>
+        <v>365908.29457723582</v>
       </c>
       <c r="AA8" s="31">
         <f>(Calculations!AB12)*(About!$A$70)</f>
-        <v>235700.54</v>
+        <v>364030.41294300999</v>
       </c>
       <c r="AB8" s="31">
         <f>(Calculations!AC12)*(About!$A$70)</f>
-        <v>234239.185</v>
+        <v>362247.30800235737</v>
       </c>
       <c r="AC8" s="31">
         <f>(Calculations!AD12)*(About!$A$70)</f>
-        <v>232776.859</v>
+        <v>360686.24378169485</v>
       </c>
       <c r="AD8" s="31">
         <f>(Calculations!AE12)*(About!$A$70)</f>
-        <v>231314.533</v>
+        <v>358997.91553461546</v>
       </c>
       <c r="AE8" s="31">
         <f>(Calculations!AF12)*(About!$A$70)</f>
-        <v>229852.20699999999</v>
+        <v>357342.07462037972</v>
       </c>
       <c r="AF8" s="31">
         <f>(Calculations!AG12)*(About!$A$70)</f>
-        <v>228389.88099999999</v>
+        <v>355591.4570125707</v>
       </c>
       <c r="AG8" s="31">
         <f>(Calculations!AH12)*(About!$A$70)</f>
-        <v>226927.55499999999</v>
+        <v>353524.0219911983</v>
       </c>
       <c r="AH8" s="31"/>
       <c r="AI8" s="31"/>
@@ -39363,7 +39363,7 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B15" s="31">
         <f t="shared" ref="B15:C15" si="0">B11</f>
@@ -39498,7 +39498,7 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B16" s="31">
         <f t="shared" ref="B16:C16" si="2">B11</f>
@@ -39633,7 +39633,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B17" s="31">
         <v>0</v>

</xml_diff>

<commit_message>
File updates from RMI through 12/4
</commit_message>
<xml_diff>
--- a/InputData/fuels/BS/BAU Subsidies.xlsx
+++ b/InputData/fuels/BS/BAU Subsidies.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\fuels\BS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-colorado\InputData\fuels\BS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1236,9 +1236,6 @@
     <t>offshore wind ($/MW)</t>
   </si>
   <si>
-    <t>Model output, due to endogenous learning</t>
-  </si>
-  <si>
     <t>Solar PV  - $/MW</t>
   </si>
   <si>
@@ -1915,6 +1912,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Petroleum Products (billion 2019 dollars)</t>
+  </si>
+  <si>
+    <t>See elec/CCaMC</t>
   </si>
 </sst>
 </file>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.45">
@@ -2933,12 +2933,12 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="44" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
@@ -3836,7 +3836,7 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5148,7 +5148,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="46" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C1" s="49">
         <v>2019</v>
@@ -5256,10 +5256,10 @@
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="48" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
@@ -5267,23 +5267,23 @@
     </row>
     <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="48" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48"/>
       <c r="G4" s="48" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="48" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48"/>
@@ -5291,11 +5291,11 @@
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="48" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="48" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
@@ -5305,7 +5305,7 @@
     <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="45" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>43</v>
@@ -5417,7 +5417,7 @@
         <v>45</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -5532,7 +5532,7 @@
     </row>
     <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="45" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B16" s="52" t="s">
         <v>48</v>
@@ -5639,7 +5639,7 @@
     </row>
     <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="45" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B17" s="52" t="s">
         <v>49</v>
@@ -5746,7 +5746,7 @@
     </row>
     <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="45" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B18" s="52" t="s">
         <v>50</v>
@@ -5853,7 +5853,7 @@
     </row>
     <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="45" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B19" s="52" t="s">
         <v>51</v>
@@ -5960,7 +5960,7 @@
     </row>
     <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="45" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B20" s="52" t="s">
         <v>52</v>
@@ -6067,7 +6067,7 @@
     </row>
     <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="45" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B21" s="52" t="s">
         <v>236</v>
@@ -6174,7 +6174,7 @@
     </row>
     <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="45" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B22" s="52" t="s">
         <v>53</v>
@@ -6281,7 +6281,7 @@
     </row>
     <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="45" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B23" s="52" t="s">
         <v>54</v>
@@ -6388,7 +6388,7 @@
     </row>
     <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="45" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B24" s="52" t="s">
         <v>55</v>
@@ -6495,7 +6495,7 @@
     </row>
     <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="45" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B25" s="51" t="s">
         <v>56</v>
@@ -6607,7 +6607,7 @@
     </row>
     <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="45" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B28" s="52" t="s">
         <v>58</v>
@@ -6714,7 +6714,7 @@
     </row>
     <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="45" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B29" s="52" t="s">
         <v>59</v>
@@ -6821,7 +6821,7 @@
     </row>
     <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="45" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B30" s="52" t="s">
         <v>64</v>
@@ -6928,10 +6928,10 @@
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="45" t="s">
+        <v>416</v>
+      </c>
+      <c r="B31" s="52" t="s">
         <v>417</v>
-      </c>
-      <c r="B31" s="52" t="s">
-        <v>418</v>
       </c>
       <c r="C31" s="53">
         <v>0.29147099999999998</v>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B32" s="51" t="s">
         <v>56</v>
@@ -7148,10 +7148,10 @@
     </row>
     <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="45" t="s">
+        <v>419</v>
+      </c>
+      <c r="B35" s="52" t="s">
         <v>420</v>
-      </c>
-      <c r="B35" s="52" t="s">
-        <v>421</v>
       </c>
       <c r="C35" s="53">
         <v>16.702090999999999</v>
@@ -7255,7 +7255,7 @@
     </row>
     <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="45" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B36" s="52" t="s">
         <v>64</v>
@@ -7362,7 +7362,7 @@
     </row>
     <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B37" s="52" t="s">
         <v>61</v>
@@ -7469,7 +7469,7 @@
     </row>
     <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B38" s="51" t="s">
         <v>56</v>
@@ -7577,10 +7577,10 @@
     <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="45" t="s">
+        <v>424</v>
+      </c>
+      <c r="B40" s="51" t="s">
         <v>425</v>
-      </c>
-      <c r="B40" s="51" t="s">
-        <v>426</v>
       </c>
       <c r="C40" s="55">
         <v>2.0051730000000001</v>
@@ -7690,10 +7690,10 @@
     </row>
     <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="45" t="s">
+        <v>426</v>
+      </c>
+      <c r="B43" s="52" t="s">
         <v>427</v>
-      </c>
-      <c r="B43" s="52" t="s">
-        <v>428</v>
       </c>
       <c r="C43" s="53">
         <v>38.035392999999999</v>
@@ -7797,7 +7797,7 @@
     </row>
     <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="45" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B44" s="52" t="s">
         <v>64</v>
@@ -7904,10 +7904,10 @@
     </row>
     <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="45" t="s">
+        <v>429</v>
+      </c>
+      <c r="B45" s="52" t="s">
         <v>430</v>
-      </c>
-      <c r="B45" s="52" t="s">
-        <v>431</v>
       </c>
       <c r="C45" s="53">
         <v>11.249905999999999</v>
@@ -8011,7 +8011,7 @@
     </row>
     <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="45" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B46" s="52" t="s">
         <v>52</v>
@@ -8118,7 +8118,7 @@
     </row>
     <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B47" s="52" t="s">
         <v>236</v>
@@ -8225,10 +8225,10 @@
     </row>
     <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="45" t="s">
+        <v>433</v>
+      </c>
+      <c r="B48" s="52" t="s">
         <v>434</v>
-      </c>
-      <c r="B48" s="52" t="s">
-        <v>435</v>
       </c>
       <c r="C48" s="53">
         <v>3.2253970000000001</v>
@@ -8332,7 +8332,7 @@
     </row>
     <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B49" s="52" t="s">
         <v>54</v>
@@ -8439,10 +8439,10 @@
     </row>
     <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="45" t="s">
+        <v>436</v>
+      </c>
+      <c r="B50" s="52" t="s">
         <v>437</v>
-      </c>
-      <c r="B50" s="52" t="s">
-        <v>438</v>
       </c>
       <c r="C50" s="53">
         <v>0.28126800000000002</v>
@@ -8546,7 +8546,7 @@
     </row>
     <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="45" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B51" s="51" t="s">
         <v>65</v>
@@ -8654,12 +8654,12 @@
     <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="51" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="45" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B54" s="52" t="s">
         <v>66</v>
@@ -8766,7 +8766,7 @@
     </row>
     <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="45" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B55" s="52" t="s">
         <v>67</v>
@@ -8873,10 +8873,10 @@
     </row>
     <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="45" t="s">
+        <v>441</v>
+      </c>
+      <c r="B56" s="52" t="s">
         <v>442</v>
-      </c>
-      <c r="B56" s="52" t="s">
-        <v>443</v>
       </c>
       <c r="C56" s="53">
         <v>2.5672429999999999</v>
@@ -8980,10 +8980,10 @@
     </row>
     <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="45" t="s">
+        <v>443</v>
+      </c>
+      <c r="B57" s="52" t="s">
         <v>444</v>
-      </c>
-      <c r="B57" s="52" t="s">
-        <v>445</v>
       </c>
       <c r="C57" s="58">
         <v>34.304488999999997</v>
@@ -9087,10 +9087,10 @@
     </row>
     <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="45" t="s">
+        <v>445</v>
+      </c>
+      <c r="B58" s="52" t="s">
         <v>446</v>
-      </c>
-      <c r="B58" s="52" t="s">
-        <v>447</v>
       </c>
       <c r="C58" s="53">
         <v>1.7060120000000001</v>
@@ -9194,10 +9194,10 @@
     </row>
     <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="45" t="s">
+        <v>447</v>
+      </c>
+      <c r="B59" s="52" t="s">
         <v>448</v>
-      </c>
-      <c r="B59" s="52" t="s">
-        <v>449</v>
       </c>
       <c r="C59" s="53">
         <v>2.1898119999999999</v>
@@ -9301,7 +9301,7 @@
     </row>
     <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="45" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B60" s="52" t="s">
         <v>68</v>
@@ -9413,7 +9413,7 @@
     </row>
     <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="45" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B64" s="52" t="s">
         <v>66</v>
@@ -9520,7 +9520,7 @@
     </row>
     <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="45" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B65" s="52" t="s">
         <v>67</v>
@@ -9627,10 +9627,10 @@
     </row>
     <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="45" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B66" s="52" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C66" s="53">
         <v>2.5672429999999999</v>
@@ -9734,10 +9734,10 @@
     </row>
     <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="45" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B67" s="52" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C67" s="58">
         <v>34.304488999999997</v>
@@ -9841,10 +9841,10 @@
     </row>
     <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="45" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B68" s="52" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C68" s="53">
         <v>1.7060120000000001</v>
@@ -9948,10 +9948,10 @@
     </row>
     <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="45" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B69" s="52" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C69" s="53">
         <v>2.1898119999999999</v>
@@ -10055,7 +10055,7 @@
     </row>
     <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="45" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B70" s="52" t="s">
         <v>68</v>
@@ -10236,7 +10236,7 @@
     </row>
     <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B80" s="47" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10246,22 +10246,22 @@
     </row>
     <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B82" s="47" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B83" s="47" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B84" s="47" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B85" s="47" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="86" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10276,12 +10276,12 @@
     </row>
     <row r="88" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" s="47" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="89" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B89" s="47" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="90" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10291,12 +10291,12 @@
     </row>
     <row r="91" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B91" s="47" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="92" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B92" s="47" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="93" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10306,7 +10306,7 @@
     </row>
     <row r="94" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B94" s="47" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="95" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10316,7 +10316,7 @@
     </row>
     <row r="96" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B96" s="47" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -10326,17 +10326,17 @@
     </row>
     <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B98" s="47" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B99" s="47" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B100" s="47" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -10386,7 +10386,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="46" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C1" s="49">
         <v>2019</v>
@@ -10494,10 +10494,10 @@
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="48" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
@@ -10505,23 +10505,23 @@
     </row>
     <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="48" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48"/>
       <c r="G4" s="48" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="48" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48"/>
@@ -10529,11 +10529,11 @@
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="48" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="48" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
@@ -10543,7 +10543,7 @@
     <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="45" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>138</v>
@@ -10655,7 +10655,7 @@
         <v>45</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -10781,7 +10781,7 @@
     </row>
     <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="45" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B19" s="52" t="s">
         <v>143</v>
@@ -10888,7 +10888,7 @@
     </row>
     <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="45" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B20" s="52" t="s">
         <v>144</v>
@@ -10995,7 +10995,7 @@
     </row>
     <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="45" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B21" s="52" t="s">
         <v>145</v>
@@ -11102,7 +11102,7 @@
     </row>
     <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="45" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B22" s="52" t="s">
         <v>146</v>
@@ -11209,7 +11209,7 @@
     </row>
     <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="45" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B23" s="52" t="s">
         <v>147</v>
@@ -11316,7 +11316,7 @@
     </row>
     <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B24" s="52" t="s">
         <v>148</v>
@@ -11423,7 +11423,7 @@
     </row>
     <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="45" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B25" s="52" t="s">
         <v>149</v>
@@ -11530,7 +11530,7 @@
     </row>
     <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="45" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B26" s="51" t="s">
         <v>150</v>
@@ -11642,7 +11642,7 @@
     </row>
     <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="45" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B28" s="52" t="s">
         <v>143</v>
@@ -11749,7 +11749,7 @@
     </row>
     <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="45" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B29" s="52" t="s">
         <v>144</v>
@@ -11856,7 +11856,7 @@
     </row>
     <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="45" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B30" s="52" t="s">
         <v>152</v>
@@ -11963,7 +11963,7 @@
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="45" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B31" s="52" t="s">
         <v>153</v>
@@ -12070,10 +12070,10 @@
     </row>
     <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="45" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C32" s="57">
         <v>0.22128500000000001</v>
@@ -12177,7 +12177,7 @@
     </row>
     <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="45" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B33" s="51" t="s">
         <v>150</v>
@@ -12284,7 +12284,7 @@
     </row>
     <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="45" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B34" s="51" t="s">
         <v>238</v>
@@ -12391,7 +12391,7 @@
     </row>
     <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="45" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B35" s="52" t="s">
         <v>154</v>
@@ -12499,7 +12499,7 @@
     <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B37" s="51" t="s">
         <v>155</v>
@@ -12612,7 +12612,7 @@
     </row>
     <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="45" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B40" s="52" t="s">
         <v>143</v>
@@ -12719,7 +12719,7 @@
     </row>
     <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="45" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B41" s="52" t="s">
         <v>144</v>
@@ -12826,7 +12826,7 @@
     </row>
     <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="45" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B42" s="52" t="s">
         <v>152</v>
@@ -12933,7 +12933,7 @@
     </row>
     <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="45" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B43" s="52" t="s">
         <v>157</v>
@@ -13040,7 +13040,7 @@
     </row>
     <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="45" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B44" s="52" t="s">
         <v>158</v>
@@ -13147,7 +13147,7 @@
     </row>
     <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="45" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B45" s="52" t="s">
         <v>159</v>
@@ -13254,7 +13254,7 @@
     </row>
     <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="45" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B46" s="51" t="s">
         <v>239</v>
@@ -13361,7 +13361,7 @@
     </row>
     <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="45" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B47" s="52" t="s">
         <v>160</v>
@@ -13468,7 +13468,7 @@
     </row>
     <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="45" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B48" s="51" t="s">
         <v>161</v>
@@ -13581,7 +13581,7 @@
     </row>
     <row r="51" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="45" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B51" s="52" t="s">
         <v>143</v>
@@ -13688,7 +13688,7 @@
     </row>
     <row r="52" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="45" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B52" s="52" t="s">
         <v>144</v>
@@ -13795,7 +13795,7 @@
     </row>
     <row r="53" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="45" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B53" s="52" t="s">
         <v>152</v>
@@ -13902,7 +13902,7 @@
     </row>
     <row r="54" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="45" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B54" s="52" t="s">
         <v>146</v>
@@ -14009,7 +14009,7 @@
     </row>
     <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="45" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B55" s="52" t="s">
         <v>162</v>
@@ -14116,7 +14116,7 @@
     </row>
     <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="45" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B56" s="52" t="s">
         <v>163</v>
@@ -14223,7 +14223,7 @@
     </row>
     <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="45" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B57" s="51" t="s">
         <v>241</v>
@@ -14330,7 +14330,7 @@
     </row>
     <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="45" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B58" s="51" t="s">
         <v>164</v>
@@ -14438,7 +14438,7 @@
     <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="45" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B60" s="51" t="s">
         <v>165</v>
@@ -14551,7 +14551,7 @@
     </row>
     <row r="63" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="45" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B63" s="52" t="s">
         <v>167</v>
@@ -14658,7 +14658,7 @@
     </row>
     <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="45" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B64" s="52" t="s">
         <v>168</v>
@@ -14765,7 +14765,7 @@
     </row>
     <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B65" s="52" t="s">
         <v>169</v>
@@ -14872,7 +14872,7 @@
     </row>
     <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="45" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B66" s="52" t="s">
         <v>170</v>
@@ -14979,7 +14979,7 @@
     </row>
     <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="45" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B67" s="51" t="s">
         <v>171</v>
@@ -15086,7 +15086,7 @@
     </row>
     <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="45" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B68" s="52" t="s">
         <v>172</v>
@@ -15193,7 +15193,7 @@
     </row>
     <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="45" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B69" s="51" t="s">
         <v>173</v>
@@ -15306,12 +15306,12 @@
     </row>
     <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B72" s="51" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="73" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="45" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B73" s="52" t="s">
         <v>167</v>
@@ -15418,7 +15418,7 @@
     </row>
     <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="45" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B74" s="52" t="s">
         <v>168</v>
@@ -15525,7 +15525,7 @@
     </row>
     <row r="75" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="45" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B75" s="52" t="s">
         <v>169</v>
@@ -15632,7 +15632,7 @@
     </row>
     <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="45" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B76" s="52" t="s">
         <v>170</v>
@@ -15739,7 +15739,7 @@
     </row>
     <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="45" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B77" s="51" t="s">
         <v>175</v>
@@ -15851,7 +15851,7 @@
     </row>
     <row r="79" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="45" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B79" s="52" t="s">
         <v>167</v>
@@ -15958,7 +15958,7 @@
     </row>
     <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="45" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B80" s="52" t="s">
         <v>168</v>
@@ -16065,7 +16065,7 @@
     </row>
     <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="45" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B81" s="52" t="s">
         <v>169</v>
@@ -16172,7 +16172,7 @@
     </row>
     <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="45" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B82" s="52" t="s">
         <v>170</v>
@@ -16279,7 +16279,7 @@
     </row>
     <row r="83" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="45" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B83" s="51" t="s">
         <v>175</v>
@@ -16392,12 +16392,12 @@
     </row>
     <row r="86" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B86" s="51" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="87" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="45" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B87" s="52" t="s">
         <v>178</v>
@@ -16504,7 +16504,7 @@
     </row>
     <row r="88" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="45" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B88" s="52" t="s">
         <v>179</v>
@@ -16611,7 +16611,7 @@
     </row>
     <row r="89" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="45" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B89" s="52" t="s">
         <v>180</v>
@@ -16723,7 +16723,7 @@
     </row>
     <row r="91" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="45" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B91" s="52" t="s">
         <v>178</v>
@@ -16830,7 +16830,7 @@
     </row>
     <row r="92" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="45" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B92" s="52" t="s">
         <v>179</v>
@@ -16937,7 +16937,7 @@
     </row>
     <row r="93" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="45" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B93" s="52" t="s">
         <v>180</v>
@@ -17050,7 +17050,7 @@
     </row>
     <row r="96" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="45" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B96" s="52" t="s">
         <v>182</v>
@@ -17157,7 +17157,7 @@
     </row>
     <row r="97" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="45" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B97" s="52" t="s">
         <v>183</v>
@@ -17264,7 +17264,7 @@
     </row>
     <row r="98" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="45" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B98" s="52" t="s">
         <v>184</v>
@@ -17420,7 +17420,7 @@
     </row>
     <row r="103" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B103" s="47" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="104" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -17495,17 +17495,17 @@
     </row>
     <row r="118" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B118" s="47" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B119" s="47" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="120" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B120" s="47" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="121" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -17549,7 +17549,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="46" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C1" s="49">
         <v>2019</v>
@@ -17657,10 +17657,10 @@
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="48" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
@@ -17668,23 +17668,23 @@
     </row>
     <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="48" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="48"/>
       <c r="G4" s="48" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" s="48" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="48"/>
@@ -17692,11 +17692,11 @@
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" s="48" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="48" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
@@ -17706,7 +17706,7 @@
     <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="45" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>89</v>
@@ -17818,7 +17818,7 @@
         <v>45</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -17933,7 +17933,7 @@
     </row>
     <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="45" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B16" s="52" t="s">
         <v>93</v>
@@ -18040,7 +18040,7 @@
     </row>
     <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="45" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B17" s="52" t="s">
         <v>94</v>
@@ -18147,7 +18147,7 @@
     </row>
     <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="45" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B18" s="52" t="s">
         <v>95</v>
@@ -18254,7 +18254,7 @@
     </row>
     <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="45" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B19" s="52" t="s">
         <v>96</v>
@@ -18361,7 +18361,7 @@
     </row>
     <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="45" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B20" s="52" t="s">
         <v>97</v>
@@ -18468,7 +18468,7 @@
     </row>
     <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="45" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B21" s="52" t="s">
         <v>98</v>
@@ -18575,7 +18575,7 @@
     </row>
     <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="45" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B22" s="52" t="s">
         <v>99</v>
@@ -18682,7 +18682,7 @@
     </row>
     <row r="23" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="45" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B23" s="51" t="s">
         <v>100</v>
@@ -18790,7 +18790,7 @@
     <row r="24" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="25" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="45" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B25" s="52" t="s">
         <v>242</v>
@@ -18897,7 +18897,7 @@
     </row>
     <row r="26" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="45" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B26" s="52" t="s">
         <v>243</v>
@@ -19004,7 +19004,7 @@
     </row>
     <row r="27" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="45" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B27" s="52" t="s">
         <v>244</v>
@@ -19111,7 +19111,7 @@
     </row>
     <row r="28" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="45" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B28" s="52" t="s">
         <v>245</v>
@@ -19218,7 +19218,7 @@
     </row>
     <row r="29" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="45" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B29" s="52" t="s">
         <v>246</v>
@@ -19325,7 +19325,7 @@
     </row>
     <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="45" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B30" s="52" t="s">
         <v>247</v>
@@ -19432,7 +19432,7 @@
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="45" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B31" s="52" t="s">
         <v>248</v>
@@ -19539,7 +19539,7 @@
     </row>
     <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="45" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B32" s="52" t="s">
         <v>249</v>
@@ -19646,10 +19646,10 @@
     </row>
     <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="45" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C33" s="53">
         <v>1.0901460000000001</v>
@@ -19753,7 +19753,7 @@
     </row>
     <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="45" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B34" s="52" t="s">
         <v>250</v>
@@ -19860,7 +19860,7 @@
     </row>
     <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="45" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B35" s="52" t="s">
         <v>251</v>
@@ -19967,7 +19967,7 @@
     </row>
     <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="45" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B36" s="52" t="s">
         <v>252</v>
@@ -20074,7 +20074,7 @@
     </row>
     <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="45" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B37" s="52" t="s">
         <v>253</v>
@@ -20181,7 +20181,7 @@
     </row>
     <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="45" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B38" s="52" t="s">
         <v>254</v>
@@ -20288,7 +20288,7 @@
     </row>
     <row r="39" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="45" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B39" s="52" t="s">
         <v>251</v>
@@ -20395,7 +20395,7 @@
     </row>
     <row r="40" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="45" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B40" s="52" t="s">
         <v>252</v>
@@ -20502,7 +20502,7 @@
     </row>
     <row r="41" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="45" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B41" s="52" t="s">
         <v>253</v>
@@ -20609,7 +20609,7 @@
     </row>
     <row r="42" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="45" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B42" s="52" t="s">
         <v>255</v>
@@ -20716,7 +20716,7 @@
     </row>
     <row r="43" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="45" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B43" s="52" t="s">
         <v>251</v>
@@ -20823,7 +20823,7 @@
     </row>
     <row r="44" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="45" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B44" s="52" t="s">
         <v>252</v>
@@ -20930,7 +20930,7 @@
     </row>
     <row r="45" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="45" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B45" s="52" t="s">
         <v>253</v>
@@ -21037,7 +21037,7 @@
     </row>
     <row r="46" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="45" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B46" s="52" t="s">
         <v>256</v>
@@ -21144,7 +21144,7 @@
     </row>
     <row r="47" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="45" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B47" s="52" t="s">
         <v>257</v>
@@ -21251,7 +21251,7 @@
     </row>
     <row r="48" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="45" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B48" s="52" t="s">
         <v>258</v>
@@ -21359,7 +21359,7 @@
     <row r="49" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="50" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="45" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B50" s="51" t="s">
         <v>101</v>
@@ -21478,7 +21478,7 @@
     </row>
     <row r="55" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="45" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B55" s="52" t="s">
         <v>104</v>
@@ -21585,7 +21585,7 @@
     </row>
     <row r="56" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="45" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B56" s="52" t="s">
         <v>105</v>
@@ -21692,7 +21692,7 @@
     </row>
     <row r="57" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="45" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B57" s="52" t="s">
         <v>259</v>
@@ -21799,7 +21799,7 @@
     </row>
     <row r="58" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="45" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B58" s="52" t="s">
         <v>106</v>
@@ -21906,7 +21906,7 @@
     </row>
     <row r="59" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="45" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B59" s="52" t="s">
         <v>107</v>
@@ -22013,7 +22013,7 @@
     </row>
     <row r="60" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="45" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B60" s="52" t="s">
         <v>108</v>
@@ -22120,7 +22120,7 @@
     </row>
     <row r="61" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="45" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B61" s="52" t="s">
         <v>109</v>
@@ -22227,7 +22227,7 @@
     </row>
     <row r="62" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="45" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B62" s="52" t="s">
         <v>110</v>
@@ -22339,7 +22339,7 @@
     </row>
     <row r="64" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="45" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B64" s="52" t="s">
         <v>112</v>
@@ -22446,7 +22446,7 @@
     </row>
     <row r="65" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="45" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B65" s="52" t="s">
         <v>113</v>
@@ -22553,7 +22553,7 @@
     </row>
     <row r="66" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="45" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B66" s="52" t="s">
         <v>114</v>
@@ -22660,7 +22660,7 @@
     </row>
     <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="45" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B67" s="52" t="s">
         <v>115</v>
@@ -22767,7 +22767,7 @@
     </row>
     <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="45" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B68" s="52" t="s">
         <v>260</v>
@@ -22874,7 +22874,7 @@
     </row>
     <row r="69" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="45" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B69" s="51" t="s">
         <v>116</v>
@@ -22982,7 +22982,7 @@
     <row r="70" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="71" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="45" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B71" s="52" t="s">
         <v>261</v>
@@ -23090,7 +23090,7 @@
     <row r="72" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="73" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="45" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B73" s="52" t="s">
         <v>262</v>
@@ -23197,7 +23197,7 @@
     </row>
     <row r="74" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="45" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B74" s="52" t="s">
         <v>263</v>
@@ -23304,10 +23304,10 @@
     </row>
     <row r="75" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="45" t="s">
+        <v>580</v>
+      </c>
+      <c r="B75" s="52" t="s">
         <v>581</v>
-      </c>
-      <c r="B75" s="52" t="s">
-        <v>582</v>
       </c>
       <c r="C75" s="53">
         <v>9.2183740000000007</v>
@@ -23411,10 +23411,10 @@
     </row>
     <row r="76" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="45" t="s">
+        <v>582</v>
+      </c>
+      <c r="B76" s="52" t="s">
         <v>583</v>
-      </c>
-      <c r="B76" s="52" t="s">
-        <v>584</v>
       </c>
       <c r="C76" s="53">
         <v>8.7448569999999997</v>
@@ -23518,10 +23518,10 @@
     </row>
     <row r="77" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="45" t="s">
+        <v>584</v>
+      </c>
+      <c r="B77" s="52" t="s">
         <v>585</v>
-      </c>
-      <c r="B77" s="52" t="s">
-        <v>586</v>
       </c>
       <c r="C77" s="53">
         <v>0.47351700000000002</v>
@@ -23625,7 +23625,7 @@
     </row>
     <row r="78" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="45" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B78" s="52" t="s">
         <v>117</v>
@@ -23737,10 +23737,10 @@
     </row>
     <row r="80" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="45" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B80" s="52" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C80" s="57">
         <v>173.50422699999999</v>
@@ -23944,7 +23944,7 @@
     </row>
     <row r="96" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B96" s="47" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -23954,17 +23954,17 @@
     </row>
     <row r="98" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B98" s="47" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B99" s="47" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="100" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B100" s="47" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="101" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -24009,17 +24009,17 @@
     </row>
     <row r="109" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B109" s="47" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="110" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B110" s="47" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="111" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B111" s="47" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="112" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -24059,8 +24059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47:AH47"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -24116,7 +24116,7 @@
     </row>
     <row r="2" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="13"/>
@@ -24263,103 +24263,103 @@
         <v>304</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>395</v>
+        <v>621</v>
       </c>
       <c r="C4" s="7">
-        <v>1122140</v>
+        <v>1462790.2009077901</v>
       </c>
       <c r="D4" s="7">
-        <v>1093330</v>
+        <v>1284828.0428722501</v>
       </c>
       <c r="E4" s="7">
-        <v>1068540</v>
+        <v>1237544.2340474708</v>
       </c>
       <c r="F4" s="7">
-        <v>1046900</v>
+        <v>1190260.4252226916</v>
       </c>
       <c r="G4" s="7">
-        <v>1027790</v>
+        <v>1142976.6163979124</v>
       </c>
       <c r="H4" s="7">
-        <v>1010730</v>
+        <v>1095692.8075731331</v>
       </c>
       <c r="I4" s="8">
-        <v>995371</v>
+        <v>1048408.9987483537</v>
       </c>
       <c r="J4" s="8">
-        <v>979717</v>
+        <v>1001125.1899235747</v>
       </c>
       <c r="K4" s="8">
-        <v>965590</v>
+        <v>953841.38109879522</v>
       </c>
       <c r="L4" s="8">
-        <v>952751</v>
+        <v>906557.57227401587</v>
       </c>
       <c r="M4" s="8">
-        <v>941011</v>
+        <v>859273.76344923663</v>
       </c>
       <c r="N4" s="8">
-        <v>930219</v>
+        <v>811989.95462445728</v>
       </c>
       <c r="O4" s="8">
-        <v>920839</v>
+        <v>764706.14579967817</v>
       </c>
       <c r="P4" s="8">
-        <v>912101</v>
+        <v>757913.21727074252</v>
       </c>
       <c r="Q4" s="8">
-        <v>903931</v>
+        <v>751120.28874180699</v>
       </c>
       <c r="R4" s="8">
-        <v>896269</v>
+        <v>744327.36021287122</v>
       </c>
       <c r="S4" s="8">
-        <v>889064</v>
+        <v>737534.43168393557</v>
       </c>
       <c r="T4" s="8">
-        <v>881185</v>
+        <v>730741.50315499993</v>
       </c>
       <c r="U4" s="8">
-        <v>873806</v>
+        <v>723948.57462606428</v>
       </c>
       <c r="V4" s="8">
-        <v>866873</v>
+        <v>717155.64609712863</v>
       </c>
       <c r="W4" s="8">
-        <v>860342</v>
+        <v>710362.71756819298</v>
       </c>
       <c r="X4" s="8">
-        <v>854175</v>
+        <v>703569.78903925733</v>
       </c>
       <c r="Y4" s="8">
-        <v>848033</v>
+        <v>696776.86051032168</v>
       </c>
       <c r="Z4" s="8">
-        <v>842223</v>
+        <v>689983.93198138592</v>
       </c>
       <c r="AA4" s="8">
-        <v>836717</v>
+        <v>683191.00345245027</v>
       </c>
       <c r="AB4" s="8">
-        <v>831488</v>
+        <v>676398.07492351462</v>
       </c>
       <c r="AC4" s="8">
-        <v>826512</v>
+        <v>669605.14639457897</v>
       </c>
       <c r="AD4" s="8">
-        <v>821449</v>
+        <v>662812.21786564332</v>
       </c>
       <c r="AE4" s="8">
-        <v>816631</v>
+        <v>656019.28933670768</v>
       </c>
       <c r="AF4" s="8">
-        <v>812038</v>
+        <v>649226.36080777203</v>
       </c>
       <c r="AG4" s="8">
-        <v>807654</v>
+        <v>642433.43227883638</v>
       </c>
       <c r="AH4" s="8">
-        <v>803461</v>
+        <v>635640.50374990073</v>
       </c>
     </row>
     <row r="5" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
@@ -24501,137 +24501,137 @@
       </c>
       <c r="C6" s="31">
         <f t="shared" ref="C6:AH6" si="1">C5*C4</f>
-        <v>336642</v>
+        <v>438837.060272337</v>
       </c>
       <c r="D6" s="31">
         <f t="shared" si="1"/>
-        <v>284265.8</v>
+        <v>334055.29114678502</v>
       </c>
       <c r="E6" s="31">
         <f t="shared" si="1"/>
-        <v>235078.8</v>
+        <v>272259.73149044358</v>
       </c>
       <c r="F6" s="31">
         <f t="shared" si="1"/>
-        <v>104690</v>
+        <v>119026.04252226917</v>
       </c>
       <c r="G6" s="31">
         <f t="shared" si="1"/>
-        <v>102779</v>
+        <v>114297.66163979124</v>
       </c>
       <c r="H6" s="31">
         <f t="shared" si="1"/>
-        <v>101073</v>
+        <v>109569.28075731332</v>
       </c>
       <c r="I6" s="31">
         <f t="shared" si="1"/>
-        <v>99537.1</v>
+        <v>104840.89987483538</v>
       </c>
       <c r="J6" s="31">
         <f t="shared" si="1"/>
-        <v>97971.700000000012</v>
+        <v>100112.51899235748</v>
       </c>
       <c r="K6" s="31">
         <f t="shared" si="1"/>
-        <v>96559</v>
+        <v>95384.138109879525</v>
       </c>
       <c r="L6" s="31">
         <f t="shared" si="1"/>
-        <v>95275.1</v>
+        <v>90655.757227401598</v>
       </c>
       <c r="M6" s="31">
         <f t="shared" si="1"/>
-        <v>94101.1</v>
+        <v>85927.376344923672</v>
       </c>
       <c r="N6" s="31">
         <f t="shared" si="1"/>
-        <v>93021.900000000009</v>
+        <v>81198.995462445731</v>
       </c>
       <c r="O6" s="31">
         <f t="shared" si="1"/>
-        <v>92083.900000000009</v>
+        <v>76470.61457996782</v>
       </c>
       <c r="P6" s="31">
         <f t="shared" si="1"/>
-        <v>91210.1</v>
+        <v>75791.321727074261</v>
       </c>
       <c r="Q6" s="31">
         <f t="shared" si="1"/>
-        <v>90393.1</v>
+        <v>75112.028874180702</v>
       </c>
       <c r="R6" s="31">
         <f t="shared" si="1"/>
-        <v>89626.900000000009</v>
+        <v>74432.736021287128</v>
       </c>
       <c r="S6" s="31">
         <f t="shared" si="1"/>
-        <v>88906.400000000009</v>
+        <v>73753.443168393555</v>
       </c>
       <c r="T6" s="31">
         <f t="shared" si="1"/>
-        <v>88118.5</v>
+        <v>73074.150315499995</v>
       </c>
       <c r="U6" s="31">
         <f t="shared" si="1"/>
-        <v>87380.6</v>
+        <v>72394.857462606436</v>
       </c>
       <c r="V6" s="31">
         <f t="shared" si="1"/>
-        <v>86687.3</v>
+        <v>71715.564609712863</v>
       </c>
       <c r="W6" s="31">
         <f t="shared" si="1"/>
-        <v>86034.200000000012</v>
+        <v>71036.271756819304</v>
       </c>
       <c r="X6" s="31">
         <f t="shared" si="1"/>
-        <v>85417.5</v>
+        <v>70356.97890392573</v>
       </c>
       <c r="Y6" s="31">
         <f t="shared" si="1"/>
-        <v>84803.3</v>
+        <v>69677.686051032171</v>
       </c>
       <c r="Z6" s="31">
         <f t="shared" si="1"/>
-        <v>84222.3</v>
+        <v>68998.393198138598</v>
       </c>
       <c r="AA6" s="31">
         <f t="shared" si="1"/>
-        <v>83671.700000000012</v>
+        <v>68319.100345245024</v>
       </c>
       <c r="AB6" s="31">
         <f t="shared" si="1"/>
-        <v>83148.800000000003</v>
+        <v>67639.807492351465</v>
       </c>
       <c r="AC6" s="31">
         <f t="shared" si="1"/>
-        <v>82651.200000000012</v>
+        <v>66960.514639457906</v>
       </c>
       <c r="AD6" s="31">
         <f t="shared" si="1"/>
-        <v>82144.900000000009</v>
+        <v>66281.221786564332</v>
       </c>
       <c r="AE6" s="31">
         <f t="shared" si="1"/>
-        <v>81663.100000000006</v>
+        <v>65601.928933670773</v>
       </c>
       <c r="AF6" s="31">
         <f t="shared" si="1"/>
-        <v>81203.8</v>
+        <v>64922.636080777207</v>
       </c>
       <c r="AG6" s="31">
         <f t="shared" si="1"/>
-        <v>80765.400000000009</v>
+        <v>64243.343227883641</v>
       </c>
       <c r="AH6" s="31">
         <f t="shared" si="1"/>
-        <v>80346.100000000006</v>
+        <v>63564.050374990074</v>
       </c>
     </row>
     <row r="7" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="8" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="13"/>
@@ -24776,103 +24776,103 @@
         <v>308</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>395</v>
+        <v>621</v>
       </c>
       <c r="C10" s="7">
-        <v>3652290</v>
+        <v>6831836.4795198459</v>
       </c>
       <c r="D10" s="7">
-        <v>3497620</v>
+        <v>6500515.8491650894</v>
       </c>
       <c r="E10" s="7">
-        <v>3342950</v>
+        <v>6169195.2188103329</v>
       </c>
       <c r="F10" s="7">
-        <v>3270970</v>
+        <v>5843882.7444435377</v>
       </c>
       <c r="G10" s="7">
-        <v>3198990</v>
+        <v>5630238.7966989167</v>
       </c>
       <c r="H10" s="7">
-        <v>3127010</v>
+        <v>5422794.6290817559</v>
       </c>
       <c r="I10" s="7">
-        <v>3055030</v>
+        <v>5233450.6532794116</v>
       </c>
       <c r="J10" s="7">
-        <v>2983060</v>
+        <v>5058216.8964543967</v>
       </c>
       <c r="K10" s="7">
-        <v>2911080</v>
+        <v>4898609.074266511</v>
       </c>
       <c r="L10" s="7">
-        <v>2839100</v>
+        <v>4753976.9239266422</v>
       </c>
       <c r="M10" s="7">
-        <v>2767120</v>
+        <v>4620219.8524136795</v>
       </c>
       <c r="N10" s="7">
-        <v>2695140</v>
+        <v>4501029.6773458235</v>
       </c>
       <c r="O10" s="7">
-        <v>2623160</v>
+        <v>4393594.5403691512</v>
       </c>
       <c r="P10" s="7">
-        <v>2608110</v>
+        <v>4297491.1596871642</v>
       </c>
       <c r="Q10" s="7">
-        <v>2593050</v>
+        <v>4212533.3580054678</v>
       </c>
       <c r="R10" s="7">
-        <v>2577990</v>
+        <v>4135494.7609418505</v>
       </c>
       <c r="S10" s="7">
-        <v>2562930</v>
+        <v>4069499.8884631144</v>
       </c>
       <c r="T10" s="7">
-        <v>2547870</v>
+        <v>4010225.5494396384</v>
       </c>
       <c r="U10" s="7">
-        <v>2532810</v>
+        <v>3958592.5068339193</v>
       </c>
       <c r="V10" s="7">
-        <v>2517760</v>
+        <v>3914721.5043390612</v>
       </c>
       <c r="W10" s="7">
-        <v>2502700</v>
+        <v>3876446.5635061474</v>
       </c>
       <c r="X10" s="7">
-        <v>2487640</v>
+        <v>3843367.6747004823</v>
       </c>
       <c r="Y10" s="7">
-        <v>2472580</v>
+        <v>3814239.6224356443</v>
       </c>
       <c r="Z10" s="7">
-        <v>2457520</v>
+        <v>3789350.4384214408</v>
       </c>
       <c r="AA10" s="7">
-        <v>2442460</v>
+        <v>3768365.5466244677</v>
       </c>
       <c r="AB10" s="7">
-        <v>2427400</v>
+        <v>3749025.879948609</v>
       </c>
       <c r="AC10" s="7">
-        <v>2412350</v>
+        <v>3730662.2863270584</v>
       </c>
       <c r="AD10" s="7">
-        <v>2397290</v>
+        <v>3714585.4148475262</v>
       </c>
       <c r="AE10" s="7">
-        <v>2382230</v>
+        <v>3697197.8942802823</v>
       </c>
       <c r="AF10" s="7">
-        <v>2367170</v>
+        <v>3680144.9497464434</v>
       </c>
       <c r="AG10" s="7">
-        <v>2352110</v>
+        <v>3662115.9321582974</v>
       </c>
       <c r="AH10" s="7">
-        <v>2337050</v>
+        <v>3640824.119373824</v>
       </c>
     </row>
     <row r="11" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
@@ -25014,136 +25014,136 @@
       </c>
       <c r="C12" s="8">
         <f t="shared" ref="C12:AH12" si="3">C11*C10</f>
-        <v>1095687</v>
+        <v>2049550.9438559536</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="3"/>
-        <v>909381.20000000007</v>
+        <v>1690134.1207829234</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" si="3"/>
-        <v>735449</v>
+        <v>1357222.9481382733</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" si="3"/>
-        <v>327097</v>
+        <v>584388.27444435377</v>
       </c>
       <c r="G12" s="8">
         <f t="shared" si="3"/>
-        <v>319899</v>
+        <v>563023.87966989167</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="3"/>
-        <v>312701</v>
+        <v>542279.46290817566</v>
       </c>
       <c r="I12" s="8">
         <f t="shared" si="3"/>
-        <v>305503</v>
+        <v>523345.06532794121</v>
       </c>
       <c r="J12" s="8">
         <f t="shared" si="3"/>
-        <v>298306</v>
+        <v>505821.68964543968</v>
       </c>
       <c r="K12" s="8">
         <f t="shared" si="3"/>
-        <v>291108</v>
+        <v>489860.9074266511</v>
       </c>
       <c r="L12" s="8">
         <f t="shared" si="3"/>
-        <v>283910</v>
+        <v>475397.69239266426</v>
       </c>
       <c r="M12" s="8">
         <f t="shared" si="3"/>
-        <v>276712</v>
+        <v>462021.98524136795</v>
       </c>
       <c r="N12" s="8">
         <f t="shared" si="3"/>
-        <v>269514</v>
+        <v>450102.96773458237</v>
       </c>
       <c r="O12" s="8">
         <f t="shared" si="3"/>
-        <v>262316</v>
+        <v>439359.45403691515</v>
       </c>
       <c r="P12" s="8">
         <f t="shared" si="3"/>
-        <v>260811</v>
+        <v>429749.11596871645</v>
       </c>
       <c r="Q12" s="8">
         <f t="shared" si="3"/>
-        <v>259305</v>
+        <v>421253.3358005468</v>
       </c>
       <c r="R12" s="8">
         <f t="shared" si="3"/>
-        <v>257799</v>
+        <v>413549.47609418508</v>
       </c>
       <c r="S12" s="8">
         <f t="shared" si="3"/>
-        <v>256293</v>
+        <v>406949.98884631146</v>
       </c>
       <c r="T12" s="8">
         <f t="shared" si="3"/>
-        <v>254787</v>
+        <v>401022.55494396389</v>
       </c>
       <c r="U12" s="8">
         <f t="shared" si="3"/>
-        <v>253281</v>
+        <v>395859.25068339193</v>
       </c>
       <c r="V12" s="8">
         <f t="shared" si="3"/>
-        <v>251776</v>
+        <v>391472.15043390612</v>
       </c>
       <c r="W12" s="8">
         <f t="shared" si="3"/>
-        <v>250270</v>
+        <v>387644.65635061474</v>
       </c>
       <c r="X12" s="8">
         <f t="shared" si="3"/>
-        <v>248764</v>
+        <v>384336.76747004827</v>
       </c>
       <c r="Y12" s="8">
         <f t="shared" si="3"/>
-        <v>247258</v>
+        <v>381423.96224356443</v>
       </c>
       <c r="Z12" s="8">
         <f t="shared" si="3"/>
-        <v>245752</v>
+        <v>378935.04384214408</v>
       </c>
       <c r="AA12" s="8">
         <f t="shared" si="3"/>
-        <v>244246</v>
+        <v>376836.55466244678</v>
       </c>
       <c r="AB12" s="8">
         <f t="shared" si="3"/>
-        <v>242740</v>
+        <v>374902.58799486095</v>
       </c>
       <c r="AC12" s="8">
         <f t="shared" si="3"/>
-        <v>241235</v>
+        <v>373066.22863270587</v>
       </c>
       <c r="AD12" s="8">
         <f t="shared" si="3"/>
-        <v>239729</v>
+        <v>371458.54148475267</v>
       </c>
       <c r="AE12" s="8">
         <f t="shared" si="3"/>
-        <v>238223</v>
+        <v>369719.78942802828</v>
       </c>
       <c r="AF12" s="8">
         <f t="shared" si="3"/>
-        <v>236717</v>
+        <v>368014.49497464439</v>
       </c>
       <c r="AG12" s="8">
         <f t="shared" si="3"/>
-        <v>235211</v>
+        <v>366211.59321582975</v>
       </c>
       <c r="AH12" s="8">
         <f t="shared" si="3"/>
-        <v>233705</v>
+        <v>364082.41193738242</v>
       </c>
     </row>
     <row r="14" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="13"/>
@@ -25656,7 +25656,7 @@
     <row r="19" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="20" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -26213,7 +26213,7 @@
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A26" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -33288,7 +33288,7 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
@@ -35223,7 +35223,7 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B18" s="28">
         <f>SUM(Calculations!C$69,Calculations!C$77,Calculations!C$85,Calculations!C$93,Calculations!C$100)</f>
@@ -35358,7 +35358,7 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B19" s="28">
         <f>SUM(Calculations!C$69,Calculations!C$77,Calculations!C$85,Calculations!C$93,Calculations!C$100)</f>
@@ -35493,7 +35493,7 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B20" s="6">
         <v>0</v>
@@ -35594,7 +35594,7 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B21" s="6">
         <v>0</v>
@@ -35695,7 +35695,7 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B22" s="6">
         <v>0</v>
@@ -35807,7 +35807,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -37431,7 +37431,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B15">
         <f>B11</f>
@@ -37566,7 +37566,7 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B16">
         <f>B11</f>
@@ -37701,7 +37701,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -38447,131 +38447,131 @@
       </c>
       <c r="B7" s="31">
         <f>(Calculations!C6)*(About!$A$70)</f>
-        <v>326879.38199999998</v>
+        <v>426110.78552443918</v>
       </c>
       <c r="C7" s="31">
         <f>(Calculations!D6)*(About!$A$70)</f>
-        <v>276022.09179999999</v>
+        <v>324367.68770352827</v>
       </c>
       <c r="D7" s="31">
         <f>(Calculations!E6)*(About!$A$70)</f>
-        <v>228261.51479999998</v>
+        <v>264364.1992772207</v>
       </c>
       <c r="E7" s="31">
         <f>(Calculations!F6)*(About!$A$70)</f>
-        <v>101653.98999999999</v>
+        <v>115574.28728912336</v>
       </c>
       <c r="F7" s="31">
         <f>(Calculations!G6)*(About!$A$70)</f>
-        <v>99798.409</v>
+        <v>110983.0294522373</v>
       </c>
       <c r="G7" s="31">
         <f>(Calculations!H6)*(About!$A$70)</f>
-        <v>98141.883000000002</v>
+        <v>106391.77161535123</v>
       </c>
       <c r="H7" s="31">
         <f>(Calculations!I6)*(About!$A$70)</f>
-        <v>96650.52410000001</v>
+        <v>101800.51377846515</v>
       </c>
       <c r="I7" s="31">
         <f>(Calculations!J6)*(About!$A$70)</f>
-        <v>95130.520700000008</v>
+        <v>97209.255941579104</v>
       </c>
       <c r="J7" s="31">
         <f>(Calculations!K6)*(About!$A$70)</f>
-        <v>93758.789000000004</v>
+        <v>92617.998104693019</v>
       </c>
       <c r="K7" s="31">
         <f>(Calculations!L6)*(About!$A$70)</f>
-        <v>92512.122100000008</v>
+        <v>88026.740267806948</v>
       </c>
       <c r="L7" s="31">
         <f>(Calculations!M6)*(About!$A$70)</f>
-        <v>91372.16810000001</v>
+        <v>83435.482430920878</v>
       </c>
       <c r="M7" s="31">
         <f>(Calculations!N6)*(About!$A$70)</f>
-        <v>90324.264900000009</v>
+        <v>78844.224594034808</v>
       </c>
       <c r="N7" s="31">
         <f>(Calculations!O6)*(About!$A$70)</f>
-        <v>89413.466899999999</v>
+        <v>74252.966757148752</v>
       </c>
       <c r="O7" s="31">
         <f>(Calculations!P6)*(About!$A$70)</f>
-        <v>88565.007100000003</v>
+        <v>73593.373396989104</v>
       </c>
       <c r="P7" s="31">
         <f>(Calculations!Q6)*(About!$A$70)</f>
-        <v>87771.700100000002</v>
+        <v>72933.780036829456</v>
       </c>
       <c r="Q7" s="31">
         <f>(Calculations!R6)*(About!$A$70)</f>
-        <v>87027.719900000011</v>
+        <v>72274.186676669793</v>
       </c>
       <c r="R7" s="31">
         <f>(Calculations!S6)*(About!$A$70)</f>
-        <v>86328.114400000006</v>
+        <v>71614.593316510145</v>
       </c>
       <c r="S7" s="31">
         <f>(Calculations!T6)*(About!$A$70)</f>
-        <v>85563.063500000004</v>
+        <v>70954.999956350497</v>
       </c>
       <c r="T7" s="31">
         <f>(Calculations!U6)*(About!$A$70)</f>
-        <v>84846.562600000005</v>
+        <v>70295.406596190849</v>
       </c>
       <c r="U7" s="31">
         <f>(Calculations!V6)*(About!$A$70)</f>
-        <v>84173.368300000002</v>
+        <v>69635.813236031187</v>
       </c>
       <c r="V7" s="31">
         <f>(Calculations!W6)*(About!$A$70)</f>
-        <v>83539.208200000008</v>
+        <v>68976.219875871539</v>
       </c>
       <c r="W7" s="31">
         <f>(Calculations!X6)*(About!$A$70)</f>
-        <v>82940.392500000002</v>
+        <v>68316.626515711876</v>
       </c>
       <c r="X7" s="31">
         <f>(Calculations!Y6)*(About!$A$70)</f>
-        <v>82344.004300000001</v>
+        <v>67657.033155552243</v>
       </c>
       <c r="Y7" s="31">
         <f>(Calculations!Z6)*(About!$A$70)</f>
-        <v>81779.853300000002</v>
+        <v>66997.43979539258</v>
       </c>
       <c r="Z7" s="31">
         <f>(Calculations!AA6)*(About!$A$70)</f>
-        <v>81245.220700000005</v>
+        <v>66337.846435232917</v>
       </c>
       <c r="AA7" s="31">
         <f>(Calculations!AB6)*(About!$A$70)</f>
-        <v>80737.484800000006</v>
+        <v>65678.253075073269</v>
       </c>
       <c r="AB7" s="31">
         <f>(Calculations!AC6)*(About!$A$70)</f>
-        <v>80254.315200000012</v>
+        <v>65018.659714913621</v>
       </c>
       <c r="AC7" s="31">
         <f>(Calculations!AD6)*(About!$A$70)</f>
-        <v>79762.697899999999</v>
+        <v>64359.066354753966</v>
       </c>
       <c r="AD7" s="31">
         <f>(Calculations!AE6)*(About!$A$70)</f>
-        <v>79294.8701</v>
+        <v>63699.472994594318</v>
       </c>
       <c r="AE7" s="31">
         <f>(Calculations!AF6)*(About!$A$70)</f>
-        <v>78848.889800000004</v>
+        <v>63039.879634434663</v>
       </c>
       <c r="AF7" s="31">
         <f>(Calculations!AG6)*(About!$A$70)</f>
-        <v>78423.203400000013</v>
+        <v>62380.286274275015</v>
       </c>
       <c r="AG7" s="31">
         <f>(Calculations!AH6)*(About!$A$70)</f>
-        <v>78016.063099999999</v>
+        <v>61720.69291411536</v>
       </c>
       <c r="AH7" s="31"/>
       <c r="AI7" s="31"/>
@@ -38582,131 +38582,131 @@
       </c>
       <c r="B8" s="31">
         <f>(Calculations!C12)*(About!$A$70)</f>
-        <v>1063912.077</v>
+        <v>1990113.9664841308</v>
       </c>
       <c r="C8" s="31">
         <f>(Calculations!D12)*(About!$A$70)</f>
-        <v>883009.14520000003</v>
+        <v>1641120.2312802186</v>
       </c>
       <c r="D8" s="31">
         <f>(Calculations!E12)*(About!$A$70)</f>
-        <v>714120.97899999993</v>
+        <v>1317863.4826422634</v>
       </c>
       <c r="E8" s="31">
         <f>(Calculations!F12)*(About!$A$70)</f>
-        <v>317611.18699999998</v>
+        <v>567441.01448546746</v>
       </c>
       <c r="F8" s="31">
         <f>(Calculations!G12)*(About!$A$70)</f>
-        <v>310621.929</v>
+        <v>546696.18715946481</v>
       </c>
       <c r="G8" s="31">
         <f>(Calculations!H12)*(About!$A$70)</f>
-        <v>303632.67099999997</v>
+        <v>526553.3584838385</v>
       </c>
       <c r="H8" s="31">
         <f>(Calculations!I12)*(About!$A$70)</f>
-        <v>296643.413</v>
+        <v>508168.05843343091</v>
       </c>
       <c r="I8" s="31">
         <f>(Calculations!J12)*(About!$A$70)</f>
-        <v>289655.12599999999</v>
+        <v>491152.8606457219</v>
       </c>
       <c r="J8" s="31">
         <f>(Calculations!K12)*(About!$A$70)</f>
-        <v>282665.86800000002</v>
+        <v>475654.9411112782</v>
       </c>
       <c r="K8" s="31">
         <f>(Calculations!L12)*(About!$A$70)</f>
-        <v>275676.61</v>
+        <v>461611.15931327699</v>
       </c>
       <c r="L8" s="31">
         <f>(Calculations!M12)*(About!$A$70)</f>
-        <v>268687.35200000001</v>
+        <v>448623.34766936826</v>
       </c>
       <c r="M8" s="31">
         <f>(Calculations!N12)*(About!$A$70)</f>
-        <v>261698.09399999998</v>
+        <v>437049.98167027946</v>
       </c>
       <c r="N8" s="31">
         <f>(Calculations!O12)*(About!$A$70)</f>
-        <v>254708.83599999998</v>
+        <v>426618.02986984461</v>
       </c>
       <c r="O8" s="31">
         <f>(Calculations!P12)*(About!$A$70)</f>
-        <v>253247.481</v>
+        <v>417286.39160562365</v>
       </c>
       <c r="P8" s="31">
         <f>(Calculations!Q12)*(About!$A$70)</f>
-        <v>251785.155</v>
+        <v>409036.98906233092</v>
       </c>
       <c r="Q8" s="31">
         <f>(Calculations!R12)*(About!$A$70)</f>
-        <v>250322.829</v>
+        <v>401556.54128745373</v>
       </c>
       <c r="R8" s="31">
         <f>(Calculations!S12)*(About!$A$70)</f>
-        <v>248860.503</v>
+        <v>395148.43916976842</v>
       </c>
       <c r="S8" s="31">
         <f>(Calculations!T12)*(About!$A$70)</f>
-        <v>247398.177</v>
+        <v>389392.90085058892</v>
       </c>
       <c r="T8" s="31">
         <f>(Calculations!U12)*(About!$A$70)</f>
-        <v>245935.851</v>
+        <v>384379.33241357357</v>
       </c>
       <c r="U8" s="31">
         <f>(Calculations!V12)*(About!$A$70)</f>
-        <v>244474.49599999998</v>
+        <v>380119.45807132282</v>
       </c>
       <c r="V8" s="31">
         <f>(Calculations!W12)*(About!$A$70)</f>
-        <v>243012.16999999998</v>
+        <v>376402.96131644689</v>
       </c>
       <c r="W8" s="31">
         <f>(Calculations!X12)*(About!$A$70)</f>
-        <v>241549.84399999998</v>
+        <v>373191.00121341686</v>
       </c>
       <c r="X8" s="31">
         <f>(Calculations!Y12)*(About!$A$70)</f>
-        <v>240087.51799999998</v>
+        <v>370362.66733850102</v>
       </c>
       <c r="Y8" s="31">
         <f>(Calculations!Z12)*(About!$A$70)</f>
-        <v>238625.19199999998</v>
+        <v>367945.92757072189</v>
       </c>
       <c r="Z8" s="31">
         <f>(Calculations!AA12)*(About!$A$70)</f>
-        <v>237162.86599999998</v>
+        <v>365908.29457723582</v>
       </c>
       <c r="AA8" s="31">
         <f>(Calculations!AB12)*(About!$A$70)</f>
-        <v>235700.54</v>
+        <v>364030.41294300999</v>
       </c>
       <c r="AB8" s="31">
         <f>(Calculations!AC12)*(About!$A$70)</f>
-        <v>234239.185</v>
+        <v>362247.30800235737</v>
       </c>
       <c r="AC8" s="31">
         <f>(Calculations!AD12)*(About!$A$70)</f>
-        <v>232776.859</v>
+        <v>360686.24378169485</v>
       </c>
       <c r="AD8" s="31">
         <f>(Calculations!AE12)*(About!$A$70)</f>
-        <v>231314.533</v>
+        <v>358997.91553461546</v>
       </c>
       <c r="AE8" s="31">
         <f>(Calculations!AF12)*(About!$A$70)</f>
-        <v>229852.20699999999</v>
+        <v>357342.07462037972</v>
       </c>
       <c r="AF8" s="31">
         <f>(Calculations!AG12)*(About!$A$70)</f>
-        <v>228389.88099999999</v>
+        <v>355591.4570125707</v>
       </c>
       <c r="AG8" s="31">
         <f>(Calculations!AH12)*(About!$A$70)</f>
-        <v>226927.55499999999</v>
+        <v>353524.0219911983</v>
       </c>
       <c r="AH8" s="31"/>
       <c r="AI8" s="31"/>
@@ -39363,7 +39363,7 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B15" s="31">
         <f t="shared" ref="B15:C15" si="0">B11</f>
@@ -39498,7 +39498,7 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B16" s="31">
         <f t="shared" ref="B16:C16" si="2">B11</f>
@@ -39633,7 +39633,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B17" s="31">
         <v>0</v>

</xml_diff>